<commit_message>
git push before windows 11 update
</commit_message>
<xml_diff>
--- a/data/enhancement-PNI/San Juan Chinook Enhanced Contribution Work Around.xlsx
+++ b/data/enhancement-PNI/San Juan Chinook Enhanced Contribution Work Around.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\Area20\A20\data\enhancement-PNI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF06030-01B1-48A6-8AC2-FF8D6B368CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3917EFC-9679-4953-B3DA-45364DE94E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{99D26236-5795-441E-B1F3-A9B23A6B67D4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{99D26236-5795-441E-B1F3-A9B23A6B67D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="86">
   <si>
     <t>Releases</t>
   </si>
@@ -1078,12 +1078,6 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1125,6 +1119,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1445,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFC1460D-2AEF-4128-ACC0-DC803AE58606}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -1459,34 +1459,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="97"/>
+      <c r="A1" s="95"/>
       <c r="B1" s="7" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="2"/>
-      <c r="E2" s="81" t="s">
+      <c r="E2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="82"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="100"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="100" t="s">
+      <c r="V2" s="98" t="s">
         <v>85</v>
       </c>
-      <c r="W2" s="100"/>
-      <c r="X2" s="100"/>
-      <c r="Y2" s="100"/>
-      <c r="Z2" s="100"/>
+      <c r="W2" s="98"/>
+      <c r="X2" s="98"/>
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="98"/>
     </row>
     <row r="3" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1587,19 +1587,19 @@
       <c r="U4">
         <v>2008</v>
       </c>
-      <c r="V4" s="99">
+      <c r="V4" s="97">
         <v>6.8493150684931503E-2</v>
       </c>
-      <c r="W4" s="99">
+      <c r="W4" s="97">
         <v>0.45205479452054792</v>
       </c>
-      <c r="X4" s="99">
+      <c r="X4" s="97">
         <v>0.1095890410958904</v>
       </c>
-      <c r="Y4" s="99">
+      <c r="Y4" s="97">
         <v>0.35616438356164382</v>
       </c>
-      <c r="Z4" s="99">
+      <c r="Z4" s="97">
         <v>1.3698630136986301E-2</v>
       </c>
     </row>
@@ -1631,11 +1631,11 @@
       <c r="U5">
         <v>2009</v>
       </c>
-      <c r="V5" s="99"/>
-      <c r="W5" s="99"/>
-      <c r="X5" s="99"/>
-      <c r="Y5" s="99"/>
-      <c r="Z5" s="99"/>
+      <c r="V5" s="97"/>
+      <c r="W5" s="97"/>
+      <c r="X5" s="97"/>
+      <c r="Y5" s="97"/>
+      <c r="Z5" s="97"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1665,11 +1665,11 @@
       <c r="U6">
         <v>2010</v>
       </c>
-      <c r="V6" s="99"/>
-      <c r="W6" s="99"/>
-      <c r="X6" s="99"/>
-      <c r="Y6" s="99"/>
-      <c r="Z6" s="99"/>
+      <c r="V6" s="97"/>
+      <c r="W6" s="97"/>
+      <c r="X6" s="97"/>
+      <c r="Y6" s="97"/>
+      <c r="Z6" s="97"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1699,11 +1699,11 @@
       <c r="U7">
         <v>2011</v>
       </c>
-      <c r="V7" s="99"/>
-      <c r="W7" s="99"/>
-      <c r="X7" s="99"/>
-      <c r="Y7" s="99"/>
-      <c r="Z7" s="99"/>
+      <c r="V7" s="97"/>
+      <c r="W7" s="97"/>
+      <c r="X7" s="97"/>
+      <c r="Y7" s="97"/>
+      <c r="Z7" s="97"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1716,68 +1716,68 @@
       <c r="D8" s="2">
         <v>2012</v>
       </c>
-      <c r="E8" s="89">
+      <c r="E8" s="87">
         <v>3</v>
       </c>
-      <c r="F8" s="89">
-        <v>0</v>
-      </c>
-      <c r="G8" s="92">
+      <c r="F8" s="87">
+        <v>0</v>
+      </c>
+      <c r="G8" s="90">
         <v>1</v>
       </c>
-      <c r="H8" s="92">
+      <c r="H8" s="90">
         <v>9</v>
       </c>
-      <c r="I8" s="92">
+      <c r="I8" s="90">
         <v>2</v>
       </c>
-      <c r="J8" s="92">
+      <c r="J8" s="90">
         <v>29</v>
       </c>
-      <c r="K8" s="92">
+      <c r="K8" s="90">
         <v>6</v>
       </c>
-      <c r="L8" s="92">
+      <c r="L8" s="90">
         <v>32</v>
       </c>
-      <c r="M8" s="92">
+      <c r="M8" s="90">
         <v>1</v>
       </c>
-      <c r="N8" s="92">
-        <v>0</v>
-      </c>
-      <c r="O8" s="92">
+      <c r="N8" s="90">
+        <v>0</v>
+      </c>
+      <c r="O8" s="90">
         <f>SUM(M8,K8,I8,G8,E8)</f>
         <v>13</v>
       </c>
-      <c r="P8" s="89">
+      <c r="P8" s="87">
         <f>SUM(N8,L8,J8,H8,F8)</f>
         <v>70</v>
       </c>
-      <c r="Q8" s="98">
+      <c r="Q8" s="96">
         <f>P8/SUM(O8:P8)</f>
         <v>0.84337349397590367</v>
       </c>
       <c r="R8" s="8"/>
-      <c r="S8" s="96" t="s">
+      <c r="S8" s="94" t="s">
         <v>80</v>
       </c>
       <c r="U8">
         <v>2012</v>
       </c>
-      <c r="V8" s="99">
+      <c r="V8" s="97">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="W8" s="99">
+      <c r="W8" s="97">
         <v>0.114</v>
       </c>
-      <c r="X8" s="99">
+      <c r="X8" s="97">
         <v>0.38600000000000001</v>
       </c>
-      <c r="Y8" s="99">
+      <c r="Y8" s="97">
         <v>0.45500000000000002</v>
       </c>
-      <c r="Z8" s="99">
+      <c r="Z8" s="97">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
@@ -1796,15 +1796,15 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="91"/>
-      <c r="J9" s="91"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
-      <c r="Q9" s="98"/>
+      <c r="Q9" s="96"/>
       <c r="R9" s="8"/>
       <c r="S9" t="s">
         <v>81</v>
@@ -1812,11 +1812,11 @@
       <c r="U9">
         <v>2013</v>
       </c>
-      <c r="V9" s="99"/>
-      <c r="W9" s="99"/>
-      <c r="X9" s="99"/>
-      <c r="Y9" s="99"/>
-      <c r="Z9" s="99"/>
+      <c r="V9" s="97"/>
+      <c r="W9" s="97"/>
+      <c r="X9" s="97"/>
+      <c r="Y9" s="97"/>
+      <c r="Z9" s="97"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1847,10 +1847,10 @@
       <c r="J10" s="8">
         <v>79</v>
       </c>
-      <c r="K10" s="90">
+      <c r="K10" s="88">
         <v>1</v>
       </c>
-      <c r="L10" s="90">
+      <c r="L10" s="88">
         <v>4</v>
       </c>
       <c r="M10" s="8">
@@ -1867,7 +1867,7 @@
         <f>SUM(F10,H10,J10,L10,N10)</f>
         <v>92</v>
       </c>
-      <c r="Q10" s="98">
+      <c r="Q10" s="96">
         <f t="shared" ref="Q10:Q18" si="0">P10/SUM(O10:P10)</f>
         <v>0.95833333333333337</v>
       </c>
@@ -1875,19 +1875,19 @@
       <c r="U10">
         <v>2014</v>
       </c>
-      <c r="V10" s="99">
-        <v>0</v>
-      </c>
-      <c r="W10" s="99">
+      <c r="V10" s="97">
+        <v>0</v>
+      </c>
+      <c r="W10" s="97">
         <v>0.11428571428571428</v>
       </c>
-      <c r="X10" s="99">
+      <c r="X10" s="97">
         <v>0.81904761904761902</v>
       </c>
-      <c r="Y10" s="99">
+      <c r="Y10" s="97">
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="Z10" s="99">
+      <c r="Z10" s="97">
         <v>0</v>
       </c>
     </row>
@@ -1926,10 +1926,10 @@
       <c r="L11" s="8">
         <v>26</v>
       </c>
-      <c r="M11" s="91">
-        <v>0</v>
-      </c>
-      <c r="N11" s="91">
+      <c r="M11" s="89">
+        <v>0</v>
+      </c>
+      <c r="N11" s="89">
         <v>0</v>
       </c>
       <c r="O11" s="9">
@@ -1940,7 +1940,7 @@
         <f t="shared" ref="P11:P18" si="2">SUM(F11,H11,J11,L11,N11)</f>
         <v>73</v>
       </c>
-      <c r="Q11" s="98">
+      <c r="Q11" s="96">
         <f t="shared" si="0"/>
         <v>0.83908045977011492</v>
       </c>
@@ -1948,19 +1948,19 @@
       <c r="U11">
         <v>2015</v>
       </c>
-      <c r="V11" s="99">
-        <v>0</v>
-      </c>
-      <c r="W11" s="99">
+      <c r="V11" s="97">
+        <v>0</v>
+      </c>
+      <c r="W11" s="97">
         <v>0.26666666666666666</v>
       </c>
-      <c r="X11" s="99">
+      <c r="X11" s="97">
         <v>0.4</v>
       </c>
-      <c r="Y11" s="99">
+      <c r="Y11" s="97">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Z11" s="99">
+      <c r="Z11" s="97">
         <v>0</v>
       </c>
     </row>
@@ -1975,8 +1975,8 @@
       <c r="D12" s="2">
         <v>2016</v>
       </c>
-      <c r="E12" s="91"/>
-      <c r="F12" s="91"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -1993,7 +1993,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="98"/>
+      <c r="Q12" s="96"/>
       <c r="R12" s="9"/>
       <c r="S12" t="s">
         <v>81</v>
@@ -2001,11 +2001,11 @@
       <c r="U12">
         <v>2016</v>
       </c>
-      <c r="V12" s="99"/>
-      <c r="W12" s="99"/>
-      <c r="X12" s="99"/>
-      <c r="Y12" s="99"/>
-      <c r="Z12" s="99"/>
+      <c r="V12" s="97"/>
+      <c r="W12" s="97"/>
+      <c r="X12" s="97"/>
+      <c r="Y12" s="97"/>
+      <c r="Z12" s="97"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -2018,16 +2018,16 @@
       <c r="D13" s="2">
         <v>2017</v>
       </c>
-      <c r="E13" s="91">
-        <v>0</v>
-      </c>
-      <c r="F13" s="91">
-        <v>0</v>
-      </c>
-      <c r="G13" s="91">
+      <c r="E13" s="89">
+        <v>0</v>
+      </c>
+      <c r="F13" s="89">
+        <v>0</v>
+      </c>
+      <c r="G13" s="89">
         <v>5</v>
       </c>
-      <c r="H13" s="91">
+      <c r="H13" s="89">
         <v>17</v>
       </c>
       <c r="I13" s="8">
@@ -2056,7 +2056,7 @@
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
-      <c r="Q13" s="98">
+      <c r="Q13" s="96">
         <f t="shared" si="0"/>
         <v>0.75862068965517238</v>
       </c>
@@ -2064,19 +2064,19 @@
       <c r="U13">
         <v>2017</v>
       </c>
-      <c r="V13" s="99">
-        <v>0</v>
-      </c>
-      <c r="W13" s="99">
+      <c r="V13" s="97">
+        <v>0</v>
+      </c>
+      <c r="W13" s="97">
         <v>0.26500000000000001</v>
       </c>
-      <c r="X13" s="99">
+      <c r="X13" s="97">
         <v>0.56100000000000005</v>
       </c>
-      <c r="Y13" s="99">
+      <c r="Y13" s="97">
         <v>0.16300000000000001</v>
       </c>
-      <c r="Z13" s="99">
+      <c r="Z13" s="97">
         <v>0.01</v>
       </c>
     </row>
@@ -2091,22 +2091,22 @@
       <c r="D14" s="2">
         <v>2018</v>
       </c>
-      <c r="E14" s="91">
-        <v>0</v>
-      </c>
-      <c r="F14" s="91">
+      <c r="E14" s="89">
+        <v>0</v>
+      </c>
+      <c r="F14" s="89">
         <v>1</v>
       </c>
-      <c r="G14" s="91">
+      <c r="G14" s="89">
         <v>4</v>
       </c>
-      <c r="H14" s="91">
+      <c r="H14" s="89">
         <v>9</v>
       </c>
-      <c r="I14" s="91">
+      <c r="I14" s="89">
         <v>1</v>
       </c>
-      <c r="J14" s="91">
+      <c r="J14" s="89">
         <v>2</v>
       </c>
       <c r="K14" s="8">
@@ -2129,7 +2129,7 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="Q14" s="98">
+      <c r="Q14" s="96">
         <f t="shared" si="0"/>
         <v>0.72727272727272729</v>
       </c>
@@ -2137,19 +2137,19 @@
       <c r="U14">
         <v>2018</v>
       </c>
-      <c r="V14" s="99">
+      <c r="V14" s="97">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="W14" s="99">
+      <c r="W14" s="97">
         <v>0.58299999999999996</v>
       </c>
-      <c r="X14" s="99">
+      <c r="X14" s="97">
         <v>0.16700000000000001</v>
       </c>
-      <c r="Y14" s="99">
+      <c r="Y14" s="97">
         <v>0.20799999999999999</v>
       </c>
-      <c r="Z14" s="99">
+      <c r="Z14" s="97">
         <v>0</v>
       </c>
     </row>
@@ -2164,28 +2164,28 @@
       <c r="D15" s="2">
         <v>2019</v>
       </c>
-      <c r="E15" s="91">
-        <v>0</v>
-      </c>
-      <c r="F15" s="91">
-        <v>0</v>
-      </c>
-      <c r="G15" s="91">
+      <c r="E15" s="89">
+        <v>0</v>
+      </c>
+      <c r="F15" s="89">
+        <v>0</v>
+      </c>
+      <c r="G15" s="89">
         <v>1</v>
       </c>
-      <c r="H15" s="91">
+      <c r="H15" s="89">
         <v>33</v>
       </c>
-      <c r="I15" s="91">
+      <c r="I15" s="89">
         <v>19</v>
       </c>
-      <c r="J15" s="91">
+      <c r="J15" s="89">
         <v>42</v>
       </c>
-      <c r="K15" s="91">
-        <v>0</v>
-      </c>
-      <c r="L15" s="91">
+      <c r="K15" s="89">
+        <v>0</v>
+      </c>
+      <c r="L15" s="89">
         <v>1</v>
       </c>
       <c r="M15" s="8">
@@ -2202,7 +2202,7 @@
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="Q15" s="98">
+      <c r="Q15" s="96">
         <f t="shared" si="0"/>
         <v>0.79166666666666663</v>
       </c>
@@ -2210,19 +2210,19 @@
       <c r="U15">
         <v>2019</v>
       </c>
-      <c r="V15" s="99">
-        <v>0</v>
-      </c>
-      <c r="W15" s="99">
+      <c r="V15" s="97">
+        <v>0</v>
+      </c>
+      <c r="W15" s="97">
         <v>0.371</v>
       </c>
-      <c r="X15" s="99">
+      <c r="X15" s="97">
         <v>0.61</v>
       </c>
-      <c r="Y15" s="99">
+      <c r="Y15" s="97">
         <v>1.9E-2</v>
       </c>
-      <c r="Z15" s="99">
+      <c r="Z15" s="97">
         <v>0</v>
       </c>
     </row>
@@ -2243,28 +2243,28 @@
       <c r="F16" s="8">
         <v>0</v>
       </c>
-      <c r="G16" s="91">
+      <c r="G16" s="89">
         <v>5</v>
       </c>
-      <c r="H16" s="91">
+      <c r="H16" s="89">
         <v>23</v>
       </c>
-      <c r="I16" s="91">
+      <c r="I16" s="89">
         <v>14</v>
       </c>
-      <c r="J16" s="91">
+      <c r="J16" s="89">
         <v>150</v>
       </c>
-      <c r="K16" s="91">
+      <c r="K16" s="89">
         <v>12</v>
       </c>
-      <c r="L16" s="91">
+      <c r="L16" s="89">
         <v>14</v>
       </c>
-      <c r="M16" s="91">
-        <v>0</v>
-      </c>
-      <c r="N16" s="91">
+      <c r="M16" s="89">
+        <v>0</v>
+      </c>
+      <c r="N16" s="89">
         <v>0</v>
       </c>
       <c r="O16" s="9">
@@ -2275,7 +2275,7 @@
         <f t="shared" si="2"/>
         <v>187</v>
       </c>
-      <c r="Q16" s="98">
+      <c r="Q16" s="96">
         <f t="shared" si="0"/>
         <v>0.85779816513761464</v>
       </c>
@@ -2283,19 +2283,19 @@
       <c r="U16">
         <v>2020</v>
       </c>
-      <c r="V16" s="99">
-        <v>0</v>
-      </c>
-      <c r="W16" s="99">
+      <c r="V16" s="97">
+        <v>0</v>
+      </c>
+      <c r="W16" s="97">
         <v>0.13100000000000001</v>
       </c>
-      <c r="X16" s="99">
+      <c r="X16" s="97">
         <v>0.752</v>
       </c>
-      <c r="Y16" s="99">
+      <c r="Y16" s="97">
         <v>0.11700000000000001</v>
       </c>
-      <c r="Z16" s="99">
+      <c r="Z16" s="97">
         <v>0</v>
       </c>
     </row>
@@ -2322,22 +2322,22 @@
       <c r="H17" s="8">
         <v>10</v>
       </c>
-      <c r="I17" s="91">
+      <c r="I17" s="89">
         <v>41</v>
       </c>
-      <c r="J17" s="91">
+      <c r="J17" s="89">
         <v>140</v>
       </c>
-      <c r="K17" s="91">
+      <c r="K17" s="89">
         <v>3</v>
       </c>
-      <c r="L17" s="91">
+      <c r="L17" s="89">
         <v>17</v>
       </c>
-      <c r="M17" s="91">
-        <v>0</v>
-      </c>
-      <c r="N17" s="91">
+      <c r="M17" s="89">
+        <v>0</v>
+      </c>
+      <c r="N17" s="89">
         <v>0</v>
       </c>
       <c r="O17" s="9">
@@ -2348,7 +2348,7 @@
         <f t="shared" si="2"/>
         <v>167</v>
       </c>
-      <c r="Q17" s="98">
+      <c r="Q17" s="96">
         <f t="shared" si="0"/>
         <v>0.76255707762557079</v>
       </c>
@@ -2356,19 +2356,19 @@
       <c r="U17">
         <v>2021</v>
       </c>
-      <c r="V17" s="99">
-        <v>0</v>
-      </c>
-      <c r="W17" s="99">
+      <c r="V17" s="97">
+        <v>0</v>
+      </c>
+      <c r="W17" s="97">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="X17" s="99">
+      <c r="X17" s="97">
         <v>0.81899999999999995</v>
       </c>
-      <c r="Y17" s="99">
+      <c r="Y17" s="97">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="Z17" s="99">
+      <c r="Z17" s="97">
         <v>0</v>
       </c>
     </row>
@@ -2383,10 +2383,10 @@
       <c r="D18" s="2">
         <v>2022</v>
       </c>
-      <c r="E18" s="91">
-        <v>0</v>
-      </c>
-      <c r="F18" s="91">
+      <c r="E18" s="89">
+        <v>0</v>
+      </c>
+      <c r="F18" s="89">
         <v>0</v>
       </c>
       <c r="G18" s="8">
@@ -2401,16 +2401,16 @@
       <c r="J18" s="8">
         <v>67</v>
       </c>
-      <c r="K18" s="91">
+      <c r="K18" s="89">
         <v>18</v>
       </c>
-      <c r="L18" s="91">
+      <c r="L18" s="89">
         <v>29</v>
       </c>
-      <c r="M18" s="91">
+      <c r="M18" s="89">
         <v>1</v>
       </c>
-      <c r="N18" s="91">
+      <c r="N18" s="89">
         <v>0</v>
       </c>
       <c r="O18" s="9">
@@ -2421,7 +2421,7 @@
         <f t="shared" si="2"/>
         <v>179</v>
       </c>
-      <c r="Q18" s="98">
+      <c r="Q18" s="96">
         <f t="shared" si="0"/>
         <v>0.63475177304964536</v>
       </c>
@@ -2429,19 +2429,19 @@
       <c r="U18">
         <v>2022</v>
       </c>
-      <c r="V18" s="99">
-        <v>0</v>
-      </c>
-      <c r="W18" s="99">
+      <c r="V18" s="97">
+        <v>0</v>
+      </c>
+      <c r="W18" s="97">
         <v>0.42499999999999999</v>
       </c>
-      <c r="X18" s="99">
+      <c r="X18" s="97">
         <v>0.40300000000000002</v>
       </c>
-      <c r="Y18" s="99">
+      <c r="Y18" s="97">
         <v>0.16800000000000001</v>
       </c>
-      <c r="Z18" s="99">
+      <c r="Z18" s="97">
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
@@ -2464,9 +2464,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C00CE3F-2823-4239-823D-10FD7EA48E30}">
   <dimension ref="A1:BH33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD1048576"/>
+      <selection pane="topRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2481,14 +2481,14 @@
     <col min="14" max="14" width="8.5703125" style="10" customWidth="1"/>
     <col min="15" max="15" width="8" style="10" customWidth="1"/>
     <col min="16" max="18" width="8.5703125" style="10" customWidth="1"/>
-    <col min="19" max="23" width="16" style="10" customWidth="1"/>
-    <col min="24" max="24" width="23.42578125" style="10" customWidth="1"/>
-    <col min="25" max="27" width="7.28515625" style="10" customWidth="1"/>
-    <col min="28" max="34" width="7.85546875" style="10" customWidth="1"/>
-    <col min="35" max="44" width="10.5703125" style="10" customWidth="1"/>
-    <col min="45" max="46" width="7.28515625" style="10" customWidth="1"/>
-    <col min="47" max="47" width="8" style="10" customWidth="1"/>
-    <col min="48" max="49" width="7.28515625" style="10" customWidth="1"/>
+    <col min="19" max="23" width="16" style="10" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="23.42578125" style="10" hidden="1" customWidth="1"/>
+    <col min="25" max="27" width="7.28515625" style="10" hidden="1" customWidth="1"/>
+    <col min="28" max="34" width="7.85546875" style="10" hidden="1" customWidth="1"/>
+    <col min="35" max="44" width="10.5703125" style="10" hidden="1" customWidth="1"/>
+    <col min="45" max="46" width="7.28515625" style="10" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="8" style="10" hidden="1" customWidth="1"/>
+    <col min="48" max="49" width="7.28515625" style="10" hidden="1" customWidth="1"/>
     <col min="50" max="53" width="11" style="10" customWidth="1"/>
     <col min="54" max="54" width="11.7109375" style="10" customWidth="1"/>
     <col min="55" max="56" width="11" style="10" bestFit="1" customWidth="1"/>
@@ -2504,7 +2504,7 @@
       </c>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="J3" s="83" t="s">
+      <c r="J3" s="81" t="s">
         <v>73</v>
       </c>
       <c r="Y3" s="60" t="s">
@@ -3365,7 +3365,7 @@
         <v>0.84831751509922348</v>
       </c>
       <c r="BG9" s="74">
-        <f t="shared" ref="BF9:BG9" si="6">BB9</f>
+        <f t="shared" ref="BG9" si="6">BB9</f>
         <v>0</v>
       </c>
       <c r="BH9" s="75"/>
@@ -3421,7 +3421,7 @@
         <v>2011</v>
       </c>
       <c r="O10" s="30">
-        <f t="shared" ref="O10:P21" si="8">A10-3</f>
+        <f t="shared" ref="O10:O20" si="8">A10-3</f>
         <v>2010</v>
       </c>
       <c r="P10" s="48">
@@ -3895,7 +3895,7 @@
         <v>67</v>
       </c>
       <c r="AY12" s="69">
-        <f t="shared" ref="AY12:AY19" si="15">AK12/AT12</f>
+        <f t="shared" ref="AY12:AY20" si="15">AK12/AT12</f>
         <v>0.91304347826086951</v>
       </c>
       <c r="AZ12" s="69">
@@ -5358,14 +5358,14 @@
         <v>41</v>
       </c>
       <c r="X20" s="23">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="Y20" s="28"/>
       <c r="Z20" s="28">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="AA20" s="28">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="AB20" s="28">
         <v>13</v>
@@ -5386,31 +5386,87 @@
       <c r="AH20" s="26">
         <v>0</v>
       </c>
-      <c r="AI20" s="33"/>
-      <c r="AJ20" s="34"/>
-      <c r="AK20" s="46"/>
-      <c r="AL20" s="47"/>
-      <c r="AM20" s="33"/>
-      <c r="AN20" s="34"/>
-      <c r="AO20" s="33"/>
-      <c r="AP20" s="34"/>
-      <c r="AQ20" s="46"/>
-      <c r="AR20" s="52"/>
-      <c r="AS20" s="65"/>
-      <c r="AT20" s="66"/>
-      <c r="AU20" s="66"/>
-      <c r="AV20" s="66"/>
-      <c r="AW20" s="35"/>
-      <c r="AX20" s="40"/>
-      <c r="AY20" s="53"/>
-      <c r="AZ20" s="42"/>
-      <c r="BA20" s="42"/>
-      <c r="BB20" s="43"/>
-      <c r="BC20" s="32"/>
-      <c r="BD20" s="32"/>
-      <c r="BE20" s="32"/>
-      <c r="BF20" s="32"/>
-      <c r="BG20" s="26"/>
+      <c r="AI20" s="33">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="34">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="46">
+        <v>2</v>
+      </c>
+      <c r="AL20" s="47">
+        <v>40</v>
+      </c>
+      <c r="AM20" s="33">
+        <v>122</v>
+      </c>
+      <c r="AN20" s="34">
+        <v>6</v>
+      </c>
+      <c r="AO20" s="33">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="34">
+        <v>2</v>
+      </c>
+      <c r="AQ20" s="46">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="52">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="65">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="66">
+        <v>42</v>
+      </c>
+      <c r="AU20" s="66">
+        <v>129</v>
+      </c>
+      <c r="AV20" s="66">
+        <v>2</v>
+      </c>
+      <c r="AW20" s="35">
+        <v>0</v>
+      </c>
+      <c r="AX20" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY20" s="70">
+        <f t="shared" si="15"/>
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="AZ20" s="69">
+        <f t="shared" ref="AZ20" si="20">AM20/AU20</f>
+        <v>0.94573643410852715</v>
+      </c>
+      <c r="BA20" s="69">
+        <f t="shared" ref="BA20" si="21">AO20/AV20</f>
+        <v>0</v>
+      </c>
+      <c r="BB20" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="BC20" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD20" s="49">
+        <f>AVERAGE(BD14:BD17,BD11)</f>
+        <v>0.76532791169865066</v>
+      </c>
+      <c r="BE20" s="32">
+        <f>AZ20</f>
+        <v>0.94573643410852715</v>
+      </c>
+      <c r="BF20" s="32">
+        <f>BF16*G20/G16</f>
+        <v>0.16750846394984323</v>
+      </c>
+      <c r="BG20" s="74" t="s">
+        <v>67</v>
+      </c>
       <c r="BH20" s="75"/>
     </row>
     <row r="21" spans="1:60" x14ac:dyDescent="0.2">
@@ -6193,7 +6249,7 @@
       <c r="G3" s="59"/>
       <c r="H3" s="36"/>
       <c r="I3" s="59"/>
-      <c r="J3" s="84" t="s">
+      <c r="J3" s="82" t="s">
         <v>73</v>
       </c>
       <c r="K3" s="59"/>
@@ -7156,7 +7212,7 @@
         <f>BB9</f>
         <v>0</v>
       </c>
-      <c r="BH9" s="85">
+      <c r="BH9" s="83">
         <f>SUM(AI9:AJ9)*BC9</f>
         <v>0</v>
       </c>
@@ -7164,35 +7220,35 @@
         <f>SUM(AI9:AJ9)-BH9</f>
         <v>3</v>
       </c>
-      <c r="BJ9" s="85">
+      <c r="BJ9" s="83">
         <f>SUM(AK9:AL9)*BD9</f>
         <v>9.1671796261049661</v>
       </c>
-      <c r="BK9" s="86">
+      <c r="BK9" s="84">
         <f>SUM(AK9:AL9)-BJ9</f>
         <v>0.83282037389503394</v>
       </c>
-      <c r="BL9" s="93">
+      <c r="BL9" s="91">
         <f>SUM(AM9:AN9)*BE9</f>
         <v>29.293484668241156</v>
       </c>
-      <c r="BM9" s="95">
+      <c r="BM9" s="93">
         <f>SUM(AM9:AN9)-BL9</f>
         <v>1.706515331758844</v>
       </c>
-      <c r="BN9" s="93">
+      <c r="BN9" s="91">
         <f>SUM(AO9:AP9)*BF9</f>
         <v>32.236065573770489</v>
       </c>
-      <c r="BO9" s="95">
+      <c r="BO9" s="93">
         <f>SUM(AO9:AP9)-BN9</f>
         <v>5.7639344262295111</v>
       </c>
-      <c r="BP9" s="93">
+      <c r="BP9" s="91">
         <f>SUM(AQ9:AR9)*BG9</f>
         <v>0</v>
       </c>
-      <c r="BQ9" s="94">
+      <c r="BQ9" s="92">
         <f>SUM(AQ9:AR9)-BP9</f>
         <v>1</v>
       </c>
@@ -7378,10 +7434,10 @@
       <c r="BK10" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="BL10" s="85" t="s">
-        <v>57</v>
-      </c>
-      <c r="BM10" s="86" t="s">
+      <c r="BL10" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="BM10" s="84" t="s">
         <v>57</v>
       </c>
       <c r="BN10" s="33" t="s">
@@ -7610,11 +7666,11 @@
       <c r="BM11" s="34">
         <v>2</v>
       </c>
-      <c r="BN11" s="85">
+      <c r="BN11" s="83">
         <f>SUM(AO11:AP11)*BF11</f>
         <v>4.0389970660737253</v>
       </c>
-      <c r="BO11" s="86">
+      <c r="BO11" s="84">
         <f>SUM(AO11:AP11)-BN11</f>
         <v>0.96100293392627467</v>
       </c>
@@ -7845,10 +7901,10 @@
         <f>AP12</f>
         <v>4</v>
       </c>
-      <c r="BP12" s="85">
-        <v>0</v>
-      </c>
-      <c r="BQ12" s="87">
+      <c r="BP12" s="83">
+        <v>0</v>
+      </c>
+      <c r="BQ12" s="85">
         <v>0</v>
       </c>
     </row>
@@ -8021,10 +8077,10 @@
       <c r="BG13" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="BH13" s="85" t="s">
-        <v>57</v>
-      </c>
-      <c r="BI13" s="86" t="s">
+      <c r="BH13" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI13" s="84" t="s">
         <v>57</v>
       </c>
       <c r="BJ13" s="33" t="s">
@@ -8223,7 +8279,7 @@
         <v>0.75471698113207553</v>
       </c>
       <c r="BA14" s="69">
-        <f t="shared" ref="BA13:BA15" si="13">AO14/SUM(AO14:AP14)</f>
+        <f t="shared" ref="BA14:BA15" si="13">AO14/SUM(AO14:AP14)</f>
         <v>0.75</v>
       </c>
       <c r="BB14" s="71" t="s">
@@ -8248,17 +8304,17 @@
         <f t="shared" si="14"/>
         <v>na</v>
       </c>
-      <c r="BH14" s="85">
-        <v>0</v>
-      </c>
-      <c r="BI14" s="86">
-        <v>0</v>
-      </c>
-      <c r="BJ14" s="85">
+      <c r="BH14" s="83">
+        <v>0</v>
+      </c>
+      <c r="BI14" s="84">
+        <v>0</v>
+      </c>
+      <c r="BJ14" s="83">
         <f>SUM(AK14:AL14)*BD14</f>
         <v>17.026519712200706</v>
       </c>
-      <c r="BK14" s="86">
+      <c r="BK14" s="84">
         <f>SUM(AK14:AL14)-BJ14</f>
         <v>4.9734802877992941</v>
       </c>
@@ -8478,27 +8534,27 @@
         <f>BB15</f>
         <v>na</v>
       </c>
-      <c r="BH15" s="85">
+      <c r="BH15" s="83">
         <f>SUM(AI15:AJ15)*BC15</f>
         <v>1</v>
       </c>
-      <c r="BI15" s="86">
+      <c r="BI15" s="84">
         <f>SUM(AI15:AJ15)-BH15</f>
         <v>0</v>
       </c>
-      <c r="BJ15" s="85">
+      <c r="BJ15" s="83">
         <f>SUM(AK15:AL15)*BD15</f>
         <v>9.2948720845778716</v>
       </c>
-      <c r="BK15" s="86">
+      <c r="BK15" s="84">
         <f>SUM(AK15:AL15)-BJ15</f>
         <v>3.7051279154221284</v>
       </c>
-      <c r="BL15" s="85">
+      <c r="BL15" s="83">
         <f>SUM(AM15:AN15)*BE15</f>
         <v>2.2068550111734782</v>
       </c>
-      <c r="BM15" s="86">
+      <c r="BM15" s="84">
         <f>SUM(AM15:AN15)-BL15</f>
         <v>0.79314498882652185</v>
       </c>
@@ -8709,33 +8765,33 @@
         <f>BB16</f>
         <v>na</v>
       </c>
-      <c r="BH16" s="85">
-        <v>0</v>
-      </c>
-      <c r="BI16" s="86">
-        <v>0</v>
-      </c>
-      <c r="BJ16" s="85">
+      <c r="BH16" s="83">
+        <v>0</v>
+      </c>
+      <c r="BI16" s="84">
+        <v>0</v>
+      </c>
+      <c r="BJ16" s="83">
         <f>AK16+(AL16*BD16)</f>
         <v>33.105406178489702</v>
       </c>
-      <c r="BK16" s="86">
+      <c r="BK16" s="84">
         <f>SUM(AK16:AL16)-BJ16</f>
         <v>0.89459382151029843</v>
       </c>
-      <c r="BL16" s="85">
+      <c r="BL16" s="83">
         <f>AM16+(AN16*BE16)</f>
         <v>42.416440294303193</v>
       </c>
-      <c r="BM16" s="86">
+      <c r="BM16" s="84">
         <f>SUM(AM16:AN16)-BL16</f>
         <v>18.583559705696807</v>
       </c>
-      <c r="BN16" s="85">
+      <c r="BN16" s="83">
         <f>SUM(AO16:AP16)*BF16</f>
         <v>0.59544827586206894</v>
       </c>
-      <c r="BO16" s="86">
+      <c r="BO16" s="84">
         <f>SUM(AO16:AP16)-BN16</f>
         <v>0.40455172413793106</v>
       </c>
@@ -8944,34 +9000,34 @@
       <c r="BI17" s="34">
         <v>0</v>
       </c>
-      <c r="BJ17" s="85">
+      <c r="BJ17" s="83">
         <f>SUM(AK17:AL17)*BD17</f>
         <v>22.807675016829265</v>
       </c>
-      <c r="BK17" s="86">
+      <c r="BK17" s="84">
         <f>SUM(AK17:AL17)-BJ17</f>
         <v>5.1923249831707352</v>
       </c>
-      <c r="BL17" s="85">
+      <c r="BL17" s="83">
         <f>SUM(AM17:AN17)*BE17</f>
         <v>149.99334952840741</v>
       </c>
-      <c r="BM17" s="86">
+      <c r="BM17" s="84">
         <f>SUM(AM17:AN17)-BL17</f>
         <v>14.006650471592593</v>
       </c>
-      <c r="BN17" s="85">
+      <c r="BN17" s="83">
         <f>SUM(AO17:AP17)*BF17</f>
         <v>14.302575548589344</v>
       </c>
-      <c r="BO17" s="86">
+      <c r="BO17" s="84">
         <f>SUM(AO17:AP17)-BN17</f>
         <v>11.697424451410656</v>
       </c>
-      <c r="BP17" s="85">
-        <v>0</v>
-      </c>
-      <c r="BQ17" s="87">
+      <c r="BP17" s="83">
+        <v>0</v>
+      </c>
+      <c r="BQ17" s="85">
         <v>0</v>
       </c>
     </row>
@@ -9182,26 +9238,26 @@
         <f>AL18</f>
         <v>8</v>
       </c>
-      <c r="BL18" s="85">
+      <c r="BL18" s="83">
         <f>SUM(AM18:AN18)*BE18</f>
         <v>140.13638222270041</v>
       </c>
-      <c r="BM18" s="86">
+      <c r="BM18" s="84">
         <f>SUM(AM18:AN18)-BL18</f>
         <v>40.863617777299595</v>
       </c>
-      <c r="BN18" s="85">
+      <c r="BN18" s="83">
         <f>SUM(AO18:AP18)*BF18</f>
         <v>16.96635030198447</v>
       </c>
-      <c r="BO18" s="86">
+      <c r="BO18" s="84">
         <f>SUM(AO18:AP18)-BN18</f>
         <v>3.0336496980155303</v>
       </c>
-      <c r="BP18" s="85">
-        <v>0</v>
-      </c>
-      <c r="BQ18" s="87">
+      <c r="BP18" s="83">
+        <v>0</v>
+      </c>
+      <c r="BQ18" s="85">
         <v>0</v>
       </c>
     </row>
@@ -9404,10 +9460,10 @@
       <c r="BG19" s="74">
         <v>0</v>
       </c>
-      <c r="BH19" s="85">
-        <v>0</v>
-      </c>
-      <c r="BI19" s="86">
+      <c r="BH19" s="83">
+        <v>0</v>
+      </c>
+      <c r="BI19" s="84">
         <v>0</v>
       </c>
       <c r="BJ19" s="33">
@@ -9426,19 +9482,19 @@
         <f>AN19</f>
         <v>42</v>
       </c>
-      <c r="BN19" s="85">
+      <c r="BN19" s="83">
         <f>SUM(AO19:AP19)*BF19</f>
         <v>29.455179937304077</v>
       </c>
-      <c r="BO19" s="86">
+      <c r="BO19" s="84">
         <f>SUM(AO19:AP19)-BN19</f>
         <v>17.544820062695923</v>
       </c>
-      <c r="BP19" s="85">
+      <c r="BP19" s="83">
         <f>SUM(AQ19:AR19)*BG19</f>
         <v>0</v>
       </c>
-      <c r="BQ19" s="87">
+      <c r="BQ19" s="85">
         <f>SUM(AQ19:AR19)-BP19</f>
         <v>1</v>
       </c>
@@ -9938,7 +9994,7 @@
       <c r="BQ24" s="35"/>
     </row>
     <row r="25" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="BM25" s="88"/>
+      <c r="BM25" s="86"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P9:R9 N9:N12 P13:R14 Q10:R10 P11 R11 P12:Q12 P20:Q20 R16 P19 Q15:R15 N17:N18">

</xml_diff>

<commit_message>
update to PNI corrections
</commit_message>
<xml_diff>
--- a/data/enhancement-PNI/San Juan Chinook Enhanced Contribution Work Around.xlsx
+++ b/data/enhancement-PNI/San Juan Chinook Enhanced Contribution Work Around.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\Area20\A20\data\enhancement-PNI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3917EFC-9679-4953-B3DA-45364DE94E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50947BB-8D19-4814-B2B4-DC1D997B270F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{99D26236-5795-441E-B1F3-A9B23A6B67D4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{99D26236-5795-441E-B1F3-A9B23A6B67D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Katie Davidson:</t>
         </r>
@@ -108,7 +108,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 spius</t>
@@ -123,7 +123,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Katie Davidson:</t>
         </r>
@@ -132,7 +132,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 spius</t>
@@ -147,7 +147,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Katie Davidson:</t>
         </r>
@@ -156,7 +156,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 FIRST FULL PBT YEAR</t>
@@ -253,7 +253,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Katie Davidson:</t>
         </r>
@@ -262,7 +262,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 spius</t>
@@ -277,7 +277,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Katie Davidson:</t>
         </r>
@@ -286,7 +286,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 spius</t>
@@ -301,7 +301,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Katie Davidson:</t>
         </r>
@@ -310,7 +310,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 spius</t>
@@ -325,7 +325,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Katie Davidson:</t>
         </r>
@@ -334,7 +334,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 spius</t>
@@ -349,7 +349,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Katie Davidson:</t>
         </r>
@@ -358,7 +358,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 FIRST FULL PBT YEAR</t>
@@ -394,7 +394,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="87">
   <si>
     <t>Releases</t>
   </si>
@@ -653,6 +653,9 @@
   <si>
     <t xml:space="preserve">BROODSTOCK Age Props (all age samples, pooled sexes) </t>
   </si>
+  <si>
+    <t>From run recon files (all broodstock ages WITH stock IDs - SJ ONLY)</t>
+  </si>
 </sst>
 </file>
 
@@ -661,7 +664,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -706,19 +709,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -771,7 +761,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -787,6 +777,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,7 +868,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -893,207 +889,204 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="3" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1102,18 +1095,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1124,6 +1117,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1459,34 +1485,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="95"/>
+      <c r="A1" s="94"/>
       <c r="B1" s="7" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="2"/>
-      <c r="E2" s="99" t="s">
+      <c r="E2" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="100"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="99"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="98" t="s">
+      <c r="V2" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="W2" s="98"/>
-      <c r="X2" s="98"/>
-      <c r="Y2" s="98"/>
-      <c r="Z2" s="98"/>
+      <c r="W2" s="97"/>
+      <c r="X2" s="97"/>
+      <c r="Y2" s="97"/>
+      <c r="Z2" s="97"/>
     </row>
     <row r="3" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1587,19 +1613,19 @@
       <c r="U4">
         <v>2008</v>
       </c>
-      <c r="V4" s="97">
+      <c r="V4" s="96">
         <v>6.8493150684931503E-2</v>
       </c>
-      <c r="W4" s="97">
+      <c r="W4" s="96">
         <v>0.45205479452054792</v>
       </c>
-      <c r="X4" s="97">
+      <c r="X4" s="96">
         <v>0.1095890410958904</v>
       </c>
-      <c r="Y4" s="97">
+      <c r="Y4" s="96">
         <v>0.35616438356164382</v>
       </c>
-      <c r="Z4" s="97">
+      <c r="Z4" s="96">
         <v>1.3698630136986301E-2</v>
       </c>
     </row>
@@ -1631,11 +1657,11 @@
       <c r="U5">
         <v>2009</v>
       </c>
-      <c r="V5" s="97"/>
-      <c r="W5" s="97"/>
-      <c r="X5" s="97"/>
-      <c r="Y5" s="97"/>
-      <c r="Z5" s="97"/>
+      <c r="V5" s="96"/>
+      <c r="W5" s="96"/>
+      <c r="X5" s="96"/>
+      <c r="Y5" s="96"/>
+      <c r="Z5" s="96"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1665,11 +1691,11 @@
       <c r="U6">
         <v>2010</v>
       </c>
-      <c r="V6" s="97"/>
-      <c r="W6" s="97"/>
-      <c r="X6" s="97"/>
-      <c r="Y6" s="97"/>
-      <c r="Z6" s="97"/>
+      <c r="V6" s="96"/>
+      <c r="W6" s="96"/>
+      <c r="X6" s="96"/>
+      <c r="Y6" s="96"/>
+      <c r="Z6" s="96"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1699,11 +1725,11 @@
       <c r="U7">
         <v>2011</v>
       </c>
-      <c r="V7" s="97"/>
-      <c r="W7" s="97"/>
-      <c r="X7" s="97"/>
-      <c r="Y7" s="97"/>
-      <c r="Z7" s="97"/>
+      <c r="V7" s="96"/>
+      <c r="W7" s="96"/>
+      <c r="X7" s="96"/>
+      <c r="Y7" s="96"/>
+      <c r="Z7" s="96"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1716,68 +1742,68 @@
       <c r="D8" s="2">
         <v>2012</v>
       </c>
-      <c r="E8" s="87">
+      <c r="E8" s="86">
         <v>3</v>
       </c>
-      <c r="F8" s="87">
-        <v>0</v>
-      </c>
-      <c r="G8" s="90">
+      <c r="F8" s="86">
+        <v>0</v>
+      </c>
+      <c r="G8" s="89">
         <v>1</v>
       </c>
-      <c r="H8" s="90">
+      <c r="H8" s="89">
         <v>9</v>
       </c>
-      <c r="I8" s="90">
+      <c r="I8" s="89">
         <v>2</v>
       </c>
-      <c r="J8" s="90">
+      <c r="J8" s="89">
         <v>29</v>
       </c>
-      <c r="K8" s="90">
+      <c r="K8" s="89">
         <v>6</v>
       </c>
-      <c r="L8" s="90">
+      <c r="L8" s="89">
         <v>32</v>
       </c>
-      <c r="M8" s="90">
+      <c r="M8" s="89">
         <v>1</v>
       </c>
-      <c r="N8" s="90">
-        <v>0</v>
-      </c>
-      <c r="O8" s="90">
+      <c r="N8" s="89">
+        <v>0</v>
+      </c>
+      <c r="O8" s="89">
         <f>SUM(M8,K8,I8,G8,E8)</f>
         <v>13</v>
       </c>
-      <c r="P8" s="87">
+      <c r="P8" s="86">
         <f>SUM(N8,L8,J8,H8,F8)</f>
         <v>70</v>
       </c>
-      <c r="Q8" s="96">
+      <c r="Q8" s="95">
         <f>P8/SUM(O8:P8)</f>
         <v>0.84337349397590367</v>
       </c>
       <c r="R8" s="8"/>
-      <c r="S8" s="94" t="s">
+      <c r="S8" s="93" t="s">
         <v>80</v>
       </c>
       <c r="U8">
         <v>2012</v>
       </c>
-      <c r="V8" s="97">
+      <c r="V8" s="96">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="W8" s="97">
+      <c r="W8" s="96">
         <v>0.114</v>
       </c>
-      <c r="X8" s="97">
+      <c r="X8" s="96">
         <v>0.38600000000000001</v>
       </c>
-      <c r="Y8" s="97">
+      <c r="Y8" s="96">
         <v>0.45500000000000002</v>
       </c>
-      <c r="Z8" s="97">
+      <c r="Z8" s="96">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
@@ -1796,15 +1822,15 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
-      <c r="Q9" s="96"/>
+      <c r="Q9" s="95"/>
       <c r="R9" s="8"/>
       <c r="S9" t="s">
         <v>81</v>
@@ -1812,11 +1838,11 @@
       <c r="U9">
         <v>2013</v>
       </c>
-      <c r="V9" s="97"/>
-      <c r="W9" s="97"/>
-      <c r="X9" s="97"/>
-      <c r="Y9" s="97"/>
-      <c r="Z9" s="97"/>
+      <c r="V9" s="96"/>
+      <c r="W9" s="96"/>
+      <c r="X9" s="96"/>
+      <c r="Y9" s="96"/>
+      <c r="Z9" s="96"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1847,10 +1873,10 @@
       <c r="J10" s="8">
         <v>79</v>
       </c>
-      <c r="K10" s="88">
+      <c r="K10" s="87">
         <v>1</v>
       </c>
-      <c r="L10" s="88">
+      <c r="L10" s="87">
         <v>4</v>
       </c>
       <c r="M10" s="8">
@@ -1867,7 +1893,7 @@
         <f>SUM(F10,H10,J10,L10,N10)</f>
         <v>92</v>
       </c>
-      <c r="Q10" s="96">
+      <c r="Q10" s="95">
         <f t="shared" ref="Q10:Q18" si="0">P10/SUM(O10:P10)</f>
         <v>0.95833333333333337</v>
       </c>
@@ -1875,19 +1901,19 @@
       <c r="U10">
         <v>2014</v>
       </c>
-      <c r="V10" s="97">
-        <v>0</v>
-      </c>
-      <c r="W10" s="97">
+      <c r="V10" s="96">
+        <v>0</v>
+      </c>
+      <c r="W10" s="96">
         <v>0.11428571428571428</v>
       </c>
-      <c r="X10" s="97">
+      <c r="X10" s="96">
         <v>0.81904761904761902</v>
       </c>
-      <c r="Y10" s="97">
+      <c r="Y10" s="96">
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="Z10" s="97">
+      <c r="Z10" s="96">
         <v>0</v>
       </c>
     </row>
@@ -1926,10 +1952,10 @@
       <c r="L11" s="8">
         <v>26</v>
       </c>
-      <c r="M11" s="89">
-        <v>0</v>
-      </c>
-      <c r="N11" s="89">
+      <c r="M11" s="88">
+        <v>0</v>
+      </c>
+      <c r="N11" s="88">
         <v>0</v>
       </c>
       <c r="O11" s="9">
@@ -1940,7 +1966,7 @@
         <f t="shared" ref="P11:P18" si="2">SUM(F11,H11,J11,L11,N11)</f>
         <v>73</v>
       </c>
-      <c r="Q11" s="96">
+      <c r="Q11" s="95">
         <f t="shared" si="0"/>
         <v>0.83908045977011492</v>
       </c>
@@ -1948,19 +1974,19 @@
       <c r="U11">
         <v>2015</v>
       </c>
-      <c r="V11" s="97">
-        <v>0</v>
-      </c>
-      <c r="W11" s="97">
+      <c r="V11" s="96">
+        <v>0</v>
+      </c>
+      <c r="W11" s="96">
         <v>0.26666666666666666</v>
       </c>
-      <c r="X11" s="97">
+      <c r="X11" s="96">
         <v>0.4</v>
       </c>
-      <c r="Y11" s="97">
+      <c r="Y11" s="96">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Z11" s="97">
+      <c r="Z11" s="96">
         <v>0</v>
       </c>
     </row>
@@ -1975,8 +2001,8 @@
       <c r="D12" s="2">
         <v>2016</v>
       </c>
-      <c r="E12" s="89"/>
-      <c r="F12" s="89"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -1993,7 +2019,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="96"/>
+      <c r="Q12" s="95"/>
       <c r="R12" s="9"/>
       <c r="S12" t="s">
         <v>81</v>
@@ -2001,11 +2027,11 @@
       <c r="U12">
         <v>2016</v>
       </c>
-      <c r="V12" s="97"/>
-      <c r="W12" s="97"/>
-      <c r="X12" s="97"/>
-      <c r="Y12" s="97"/>
-      <c r="Z12" s="97"/>
+      <c r="V12" s="96"/>
+      <c r="W12" s="96"/>
+      <c r="X12" s="96"/>
+      <c r="Y12" s="96"/>
+      <c r="Z12" s="96"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -2018,16 +2044,16 @@
       <c r="D13" s="2">
         <v>2017</v>
       </c>
-      <c r="E13" s="89">
-        <v>0</v>
-      </c>
-      <c r="F13" s="89">
-        <v>0</v>
-      </c>
-      <c r="G13" s="89">
+      <c r="E13" s="88">
+        <v>0</v>
+      </c>
+      <c r="F13" s="88">
+        <v>0</v>
+      </c>
+      <c r="G13" s="88">
         <v>5</v>
       </c>
-      <c r="H13" s="89">
+      <c r="H13" s="88">
         <v>17</v>
       </c>
       <c r="I13" s="8">
@@ -2056,7 +2082,7 @@
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
-      <c r="Q13" s="96">
+      <c r="Q13" s="95">
         <f t="shared" si="0"/>
         <v>0.75862068965517238</v>
       </c>
@@ -2064,19 +2090,19 @@
       <c r="U13">
         <v>2017</v>
       </c>
-      <c r="V13" s="97">
-        <v>0</v>
-      </c>
-      <c r="W13" s="97">
+      <c r="V13" s="96">
+        <v>0</v>
+      </c>
+      <c r="W13" s="96">
         <v>0.26500000000000001</v>
       </c>
-      <c r="X13" s="97">
+      <c r="X13" s="96">
         <v>0.56100000000000005</v>
       </c>
-      <c r="Y13" s="97">
+      <c r="Y13" s="96">
         <v>0.16300000000000001</v>
       </c>
-      <c r="Z13" s="97">
+      <c r="Z13" s="96">
         <v>0.01</v>
       </c>
     </row>
@@ -2091,22 +2117,22 @@
       <c r="D14" s="2">
         <v>2018</v>
       </c>
-      <c r="E14" s="89">
-        <v>0</v>
-      </c>
-      <c r="F14" s="89">
+      <c r="E14" s="88">
+        <v>0</v>
+      </c>
+      <c r="F14" s="88">
         <v>1</v>
       </c>
-      <c r="G14" s="89">
+      <c r="G14" s="88">
         <v>4</v>
       </c>
-      <c r="H14" s="89">
+      <c r="H14" s="88">
         <v>9</v>
       </c>
-      <c r="I14" s="89">
+      <c r="I14" s="88">
         <v>1</v>
       </c>
-      <c r="J14" s="89">
+      <c r="J14" s="88">
         <v>2</v>
       </c>
       <c r="K14" s="8">
@@ -2129,7 +2155,7 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="Q14" s="96">
+      <c r="Q14" s="95">
         <f t="shared" si="0"/>
         <v>0.72727272727272729</v>
       </c>
@@ -2137,19 +2163,19 @@
       <c r="U14">
         <v>2018</v>
       </c>
-      <c r="V14" s="97">
+      <c r="V14" s="96">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="W14" s="97">
+      <c r="W14" s="96">
         <v>0.58299999999999996</v>
       </c>
-      <c r="X14" s="97">
+      <c r="X14" s="96">
         <v>0.16700000000000001</v>
       </c>
-      <c r="Y14" s="97">
+      <c r="Y14" s="96">
         <v>0.20799999999999999</v>
       </c>
-      <c r="Z14" s="97">
+      <c r="Z14" s="96">
         <v>0</v>
       </c>
     </row>
@@ -2164,28 +2190,28 @@
       <c r="D15" s="2">
         <v>2019</v>
       </c>
-      <c r="E15" s="89">
-        <v>0</v>
-      </c>
-      <c r="F15" s="89">
-        <v>0</v>
-      </c>
-      <c r="G15" s="89">
+      <c r="E15" s="88">
+        <v>0</v>
+      </c>
+      <c r="F15" s="88">
+        <v>0</v>
+      </c>
+      <c r="G15" s="88">
         <v>1</v>
       </c>
-      <c r="H15" s="89">
+      <c r="H15" s="88">
         <v>33</v>
       </c>
-      <c r="I15" s="89">
+      <c r="I15" s="88">
         <v>19</v>
       </c>
-      <c r="J15" s="89">
+      <c r="J15" s="88">
         <v>42</v>
       </c>
-      <c r="K15" s="89">
-        <v>0</v>
-      </c>
-      <c r="L15" s="89">
+      <c r="K15" s="88">
+        <v>0</v>
+      </c>
+      <c r="L15" s="88">
         <v>1</v>
       </c>
       <c r="M15" s="8">
@@ -2202,7 +2228,7 @@
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="Q15" s="96">
+      <c r="Q15" s="95">
         <f t="shared" si="0"/>
         <v>0.79166666666666663</v>
       </c>
@@ -2210,19 +2236,19 @@
       <c r="U15">
         <v>2019</v>
       </c>
-      <c r="V15" s="97">
-        <v>0</v>
-      </c>
-      <c r="W15" s="97">
+      <c r="V15" s="96">
+        <v>0</v>
+      </c>
+      <c r="W15" s="96">
         <v>0.371</v>
       </c>
-      <c r="X15" s="97">
+      <c r="X15" s="96">
         <v>0.61</v>
       </c>
-      <c r="Y15" s="97">
+      <c r="Y15" s="96">
         <v>1.9E-2</v>
       </c>
-      <c r="Z15" s="97">
+      <c r="Z15" s="96">
         <v>0</v>
       </c>
     </row>
@@ -2243,28 +2269,28 @@
       <c r="F16" s="8">
         <v>0</v>
       </c>
-      <c r="G16" s="89">
+      <c r="G16" s="88">
         <v>5</v>
       </c>
-      <c r="H16" s="89">
+      <c r="H16" s="88">
         <v>23</v>
       </c>
-      <c r="I16" s="89">
+      <c r="I16" s="88">
         <v>14</v>
       </c>
-      <c r="J16" s="89">
+      <c r="J16" s="88">
         <v>150</v>
       </c>
-      <c r="K16" s="89">
+      <c r="K16" s="88">
         <v>12</v>
       </c>
-      <c r="L16" s="89">
+      <c r="L16" s="88">
         <v>14</v>
       </c>
-      <c r="M16" s="89">
-        <v>0</v>
-      </c>
-      <c r="N16" s="89">
+      <c r="M16" s="88">
+        <v>0</v>
+      </c>
+      <c r="N16" s="88">
         <v>0</v>
       </c>
       <c r="O16" s="9">
@@ -2275,7 +2301,7 @@
         <f t="shared" si="2"/>
         <v>187</v>
       </c>
-      <c r="Q16" s="96">
+      <c r="Q16" s="95">
         <f t="shared" si="0"/>
         <v>0.85779816513761464</v>
       </c>
@@ -2283,19 +2309,19 @@
       <c r="U16">
         <v>2020</v>
       </c>
-      <c r="V16" s="97">
-        <v>0</v>
-      </c>
-      <c r="W16" s="97">
+      <c r="V16" s="96">
+        <v>0</v>
+      </c>
+      <c r="W16" s="96">
         <v>0.13100000000000001</v>
       </c>
-      <c r="X16" s="97">
+      <c r="X16" s="96">
         <v>0.752</v>
       </c>
-      <c r="Y16" s="97">
+      <c r="Y16" s="96">
         <v>0.11700000000000001</v>
       </c>
-      <c r="Z16" s="97">
+      <c r="Z16" s="96">
         <v>0</v>
       </c>
     </row>
@@ -2322,22 +2348,22 @@
       <c r="H17" s="8">
         <v>10</v>
       </c>
-      <c r="I17" s="89">
+      <c r="I17" s="88">
         <v>41</v>
       </c>
-      <c r="J17" s="89">
+      <c r="J17" s="88">
         <v>140</v>
       </c>
-      <c r="K17" s="89">
+      <c r="K17" s="88">
         <v>3</v>
       </c>
-      <c r="L17" s="89">
+      <c r="L17" s="88">
         <v>17</v>
       </c>
-      <c r="M17" s="89">
-        <v>0</v>
-      </c>
-      <c r="N17" s="89">
+      <c r="M17" s="88">
+        <v>0</v>
+      </c>
+      <c r="N17" s="88">
         <v>0</v>
       </c>
       <c r="O17" s="9">
@@ -2348,7 +2374,7 @@
         <f t="shared" si="2"/>
         <v>167</v>
       </c>
-      <c r="Q17" s="96">
+      <c r="Q17" s="95">
         <f t="shared" si="0"/>
         <v>0.76255707762557079</v>
       </c>
@@ -2356,19 +2382,19 @@
       <c r="U17">
         <v>2021</v>
       </c>
-      <c r="V17" s="97">
-        <v>0</v>
-      </c>
-      <c r="W17" s="97">
+      <c r="V17" s="96">
+        <v>0</v>
+      </c>
+      <c r="W17" s="96">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="X17" s="97">
+      <c r="X17" s="96">
         <v>0.81899999999999995</v>
       </c>
-      <c r="Y17" s="97">
+      <c r="Y17" s="96">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="Z17" s="97">
+      <c r="Z17" s="96">
         <v>0</v>
       </c>
     </row>
@@ -2383,10 +2409,10 @@
       <c r="D18" s="2">
         <v>2022</v>
       </c>
-      <c r="E18" s="89">
-        <v>0</v>
-      </c>
-      <c r="F18" s="89">
+      <c r="E18" s="88">
+        <v>0</v>
+      </c>
+      <c r="F18" s="88">
         <v>0</v>
       </c>
       <c r="G18" s="8">
@@ -2401,16 +2427,16 @@
       <c r="J18" s="8">
         <v>67</v>
       </c>
-      <c r="K18" s="89">
+      <c r="K18" s="88">
         <v>18</v>
       </c>
-      <c r="L18" s="89">
+      <c r="L18" s="88">
         <v>29</v>
       </c>
-      <c r="M18" s="89">
+      <c r="M18" s="88">
         <v>1</v>
       </c>
-      <c r="N18" s="89">
+      <c r="N18" s="88">
         <v>0</v>
       </c>
       <c r="O18" s="9">
@@ -2421,7 +2447,7 @@
         <f t="shared" si="2"/>
         <v>179</v>
       </c>
-      <c r="Q18" s="96">
+      <c r="Q18" s="95">
         <f t="shared" si="0"/>
         <v>0.63475177304964536</v>
       </c>
@@ -2429,19 +2455,19 @@
       <c r="U18">
         <v>2022</v>
       </c>
-      <c r="V18" s="97">
-        <v>0</v>
-      </c>
-      <c r="W18" s="97">
+      <c r="V18" s="96">
+        <v>0</v>
+      </c>
+      <c r="W18" s="96">
         <v>0.42499999999999999</v>
       </c>
-      <c r="X18" s="97">
+      <c r="X18" s="96">
         <v>0.40300000000000002</v>
       </c>
-      <c r="Y18" s="97">
+      <c r="Y18" s="96">
         <v>0.16800000000000001</v>
       </c>
-      <c r="Z18" s="97">
+      <c r="Z18" s="96">
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
@@ -2465,8 +2491,8 @@
   <dimension ref="A1:BH33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F28" sqref="F28"/>
+      <pane xSplit="1" topLeftCell="AQ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BB40" sqref="BB40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2481,14 +2507,14 @@
     <col min="14" max="14" width="8.5703125" style="10" customWidth="1"/>
     <col min="15" max="15" width="8" style="10" customWidth="1"/>
     <col min="16" max="18" width="8.5703125" style="10" customWidth="1"/>
-    <col min="19" max="23" width="16" style="10" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="23.42578125" style="10" hidden="1" customWidth="1"/>
-    <col min="25" max="27" width="7.28515625" style="10" hidden="1" customWidth="1"/>
-    <col min="28" max="34" width="7.85546875" style="10" hidden="1" customWidth="1"/>
-    <col min="35" max="44" width="10.5703125" style="10" hidden="1" customWidth="1"/>
-    <col min="45" max="46" width="7.28515625" style="10" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="8" style="10" hidden="1" customWidth="1"/>
-    <col min="48" max="49" width="7.28515625" style="10" hidden="1" customWidth="1"/>
+    <col min="19" max="23" width="16" style="10" customWidth="1"/>
+    <col min="24" max="24" width="23.42578125" style="10" customWidth="1"/>
+    <col min="25" max="27" width="7.28515625" style="10" customWidth="1"/>
+    <col min="28" max="34" width="7.85546875" style="10" customWidth="1"/>
+    <col min="35" max="44" width="10.5703125" style="10" customWidth="1"/>
+    <col min="45" max="46" width="7.28515625" style="10" customWidth="1"/>
+    <col min="47" max="47" width="8" style="10" customWidth="1"/>
+    <col min="48" max="49" width="7.28515625" style="10" customWidth="1"/>
     <col min="50" max="53" width="11" style="10" customWidth="1"/>
     <col min="54" max="54" width="11.7109375" style="10" customWidth="1"/>
     <col min="55" max="56" width="11" style="10" bestFit="1" customWidth="1"/>
@@ -2504,31 +2530,34 @@
       </c>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="J3" s="81" t="s">
+      <c r="J3" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="Y3" s="60" t="s">
+      <c r="Y3" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="Z3" s="59"/>
-      <c r="AA3" s="59"/>
-      <c r="AB3" s="59"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58"/>
       <c r="AC3" s="36"/>
-      <c r="AD3" s="60" t="s">
+      <c r="AD3" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="AI3" s="60" t="s">
+      <c r="AI3" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="AJ3" s="59"/>
-      <c r="AK3" s="59"/>
-      <c r="AL3" s="59"/>
-      <c r="AM3" s="59"/>
-      <c r="AN3" s="59"/>
-      <c r="AO3" s="59"/>
-      <c r="AP3" s="59"/>
-      <c r="AQ3" s="59"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58"/>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="58"/>
+      <c r="AN3" s="58"/>
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58"/>
       <c r="AR3" s="36"/>
+      <c r="AS3" s="58" t="s">
+        <v>78</v>
+      </c>
       <c r="AZ3" s="11" t="s">
         <v>63</v>
       </c>
@@ -3039,10 +3068,10 @@
       <c r="AP7" s="34"/>
       <c r="AQ7" s="33"/>
       <c r="AR7" s="35"/>
-      <c r="AS7" s="65"/>
-      <c r="AT7" s="66"/>
-      <c r="AU7" s="66"/>
-      <c r="AV7" s="66"/>
+      <c r="AS7" s="64"/>
+      <c r="AT7" s="65"/>
+      <c r="AU7" s="65"/>
+      <c r="AV7" s="65"/>
       <c r="AW7" s="35"/>
       <c r="AX7" s="40"/>
       <c r="AY7" s="41"/>
@@ -3153,10 +3182,10 @@
       <c r="AP8" s="34"/>
       <c r="AQ8" s="33"/>
       <c r="AR8" s="35"/>
-      <c r="AS8" s="65"/>
-      <c r="AT8" s="66"/>
-      <c r="AU8" s="66"/>
-      <c r="AV8" s="66"/>
+      <c r="AS8" s="64"/>
+      <c r="AT8" s="65"/>
+      <c r="AU8" s="65"/>
+      <c r="AV8" s="65"/>
       <c r="AW8" s="35"/>
       <c r="AX8" s="44"/>
       <c r="AY8" s="41"/>
@@ -3286,13 +3315,13 @@
       <c r="AI9" s="33">
         <v>0</v>
       </c>
-      <c r="AJ9" s="67">
+      <c r="AJ9" s="66">
         <v>3</v>
       </c>
       <c r="AK9" s="46">
         <v>0</v>
       </c>
-      <c r="AL9" s="68">
+      <c r="AL9" s="67">
         <v>10</v>
       </c>
       <c r="AM9" s="33">
@@ -3313,46 +3342,46 @@
       <c r="AR9" s="35">
         <v>1</v>
       </c>
-      <c r="AS9" s="65">
+      <c r="AS9" s="64">
         <v>3</v>
       </c>
-      <c r="AT9" s="66">
+      <c r="AT9" s="65">
         <v>10</v>
       </c>
-      <c r="AU9" s="66">
+      <c r="AU9" s="65">
         <v>33</v>
       </c>
-      <c r="AV9" s="66">
+      <c r="AV9" s="65">
         <v>38</v>
       </c>
       <c r="AW9" s="35">
         <v>1</v>
       </c>
-      <c r="AX9" s="69">
+      <c r="AX9" s="68">
         <f>AI9/AS9</f>
         <v>0</v>
       </c>
-      <c r="AY9" s="70">
+      <c r="AY9" s="69">
         <f>AK9/AT9</f>
         <v>0</v>
       </c>
-      <c r="AZ9" s="69">
+      <c r="AZ9" s="68">
         <f>AM9/AU9</f>
         <v>0</v>
       </c>
-      <c r="BA9" s="69">
+      <c r="BA9" s="68">
         <f>AO9/AV9</f>
         <v>0</v>
       </c>
-      <c r="BB9" s="71">
+      <c r="BB9" s="70">
         <f>AQ9/AW9</f>
         <v>0</v>
       </c>
-      <c r="BC9" s="72">
+      <c r="BC9" s="71">
         <f>AX9</f>
         <v>0</v>
       </c>
-      <c r="BD9" s="73">
+      <c r="BD9" s="72">
         <f>(SUM(BD11*E11+BD12*E12)/SUM(E11:E12))*(E9/E12)</f>
         <v>0.90091169057788012</v>
       </c>
@@ -3364,11 +3393,11 @@
         <f>SUM(BF12*G12+BF15*G15)/SUM(G12,G15)</f>
         <v>0.84831751509922348</v>
       </c>
-      <c r="BG9" s="74">
+      <c r="BG9" s="73">
         <f t="shared" ref="BG9" si="6">BB9</f>
         <v>0</v>
       </c>
-      <c r="BH9" s="75"/>
+      <c r="BH9" s="74"/>
     </row>
     <row r="10" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A10" s="21">
@@ -3494,34 +3523,34 @@
       <c r="AR10" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AS10" s="65" t="s">
-        <v>57</v>
-      </c>
-      <c r="AT10" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="AU10" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV10" s="66" t="s">
+      <c r="AS10" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT10" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU10" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV10" s="65" t="s">
         <v>57</v>
       </c>
       <c r="AW10" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AX10" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="AY10" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="AZ10" s="70" t="s">
-        <v>57</v>
-      </c>
-      <c r="BA10" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="BB10" s="71" t="s">
+      <c r="AX10" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY10" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ10" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA10" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB10" s="70" t="s">
         <v>57</v>
       </c>
       <c r="BC10" s="32" t="s">
@@ -3539,7 +3568,7 @@
       <c r="BG10" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="BH10" s="75"/>
+      <c r="BH10" s="74"/>
     </row>
     <row r="11" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A11" s="21">
@@ -3555,7 +3584,7 @@
       <c r="D11" s="21">
         <v>1031800</v>
       </c>
-      <c r="E11" s="76">
+      <c r="E11" s="75">
         <v>245000</v>
       </c>
       <c r="F11" s="21">
@@ -3681,37 +3710,37 @@
       <c r="AR11" s="35">
         <v>0</v>
       </c>
-      <c r="AS11" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="66">
+      <c r="AS11" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="65">
         <v>11</v>
       </c>
-      <c r="AU11" s="66">
+      <c r="AU11" s="65">
         <v>85</v>
       </c>
-      <c r="AV11" s="66">
+      <c r="AV11" s="65">
         <v>7</v>
       </c>
       <c r="AW11" s="35">
         <v>0</v>
       </c>
-      <c r="AX11" s="69" t="s">
+      <c r="AX11" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="AY11" s="69">
+      <c r="AY11" s="68">
         <f>AK11/AT11</f>
         <v>0.81818181818181823</v>
       </c>
-      <c r="AZ11" s="69">
+      <c r="AZ11" s="68">
         <f t="shared" ref="AZ11:AZ19" si="12">AM11/AU11</f>
         <v>0.92941176470588238</v>
       </c>
-      <c r="BA11" s="70">
+      <c r="BA11" s="69">
         <f t="shared" ref="BA11:BA19" si="13">AO11/AV11</f>
         <v>0</v>
       </c>
-      <c r="BB11" s="71" t="s">
+      <c r="BB11" s="70" t="s">
         <v>67</v>
       </c>
       <c r="BC11" s="32" t="str">
@@ -3734,7 +3763,7 @@
         <f>BB11</f>
         <v>na</v>
       </c>
-      <c r="BH11" s="75"/>
+      <c r="BH11" s="74"/>
     </row>
     <row r="12" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A12" s="21">
@@ -3750,7 +3779,7 @@
       <c r="D12" s="21">
         <v>319000</v>
       </c>
-      <c r="E12" s="76">
+      <c r="E12" s="75">
         <v>1031800</v>
       </c>
       <c r="F12" s="21">
@@ -3876,37 +3905,37 @@
       <c r="AR12" s="52">
         <v>0</v>
       </c>
-      <c r="AS12" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT12" s="66">
+      <c r="AS12" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="65">
         <v>23</v>
       </c>
-      <c r="AU12" s="66">
+      <c r="AU12" s="65">
         <v>36</v>
       </c>
-      <c r="AV12" s="66">
+      <c r="AV12" s="65">
         <v>30</v>
       </c>
       <c r="AW12" s="35">
         <v>0</v>
       </c>
-      <c r="AX12" s="69" t="s">
+      <c r="AX12" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="AY12" s="69">
+      <c r="AY12" s="68">
         <f t="shared" ref="AY12:AY20" si="15">AK12/AT12</f>
         <v>0.91304347826086951</v>
       </c>
-      <c r="AZ12" s="69">
+      <c r="AZ12" s="68">
         <f>AM12/AU12</f>
         <v>0.72222222222222221</v>
       </c>
-      <c r="BA12" s="69">
+      <c r="BA12" s="68">
         <f t="shared" si="13"/>
         <v>0.8666666666666667</v>
       </c>
-      <c r="BB12" s="77" t="s">
+      <c r="BB12" s="76" t="s">
         <v>67</v>
       </c>
       <c r="BC12" s="32" t="str">
@@ -3925,10 +3954,10 @@
         <f t="shared" ref="BF12" si="16">BA12</f>
         <v>0.8666666666666667</v>
       </c>
-      <c r="BG12" s="74" t="s">
+      <c r="BG12" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="BH12" s="75"/>
+      <c r="BH12" s="74"/>
     </row>
     <row r="13" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A13" s="21">
@@ -4054,34 +4083,34 @@
       <c r="AR13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AS13" s="65" t="s">
-        <v>57</v>
-      </c>
-      <c r="AT13" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="AU13" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV13" s="66" t="s">
+      <c r="AS13" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT13" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU13" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV13" s="65" t="s">
         <v>57</v>
       </c>
       <c r="AW13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AX13" s="70" t="s">
-        <v>57</v>
-      </c>
-      <c r="AY13" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="AZ13" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="BA13" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="BB13" s="71" t="s">
+      <c r="AX13" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY13" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ13" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA13" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB13" s="70" t="s">
         <v>57</v>
       </c>
       <c r="BC13" s="49" t="s">
@@ -4099,7 +4128,7 @@
       <c r="BG13" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="BH13" s="75"/>
+      <c r="BH13" s="74"/>
     </row>
     <row r="14" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A14" s="21">
@@ -4243,43 +4272,43 @@
       <c r="AR14" s="35">
         <v>0</v>
       </c>
-      <c r="AS14" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT14" s="66">
+      <c r="AS14" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="65">
         <v>25</v>
       </c>
-      <c r="AU14" s="66">
+      <c r="AU14" s="65">
         <v>53</v>
       </c>
-      <c r="AV14" s="66">
+      <c r="AV14" s="65">
         <v>15</v>
       </c>
       <c r="AW14" s="35">
         <v>1</v>
       </c>
-      <c r="AX14" s="70" t="s">
+      <c r="AX14" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="AY14" s="70">
+      <c r="AY14" s="69">
         <f t="shared" si="15"/>
         <v>0.12</v>
       </c>
-      <c r="AZ14" s="69">
+      <c r="AZ14" s="68">
         <f>AM14/AU14</f>
         <v>0.75471698113207553</v>
       </c>
-      <c r="BA14" s="69">
+      <c r="BA14" s="68">
         <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
-      <c r="BB14" s="71" t="s">
+      <c r="BB14" s="70" t="s">
         <v>67</v>
       </c>
       <c r="BC14" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="BD14" s="73">
+      <c r="BD14" s="72">
         <f>SUM(BD11*E11+BD19*E19)/SUM(E11,E19)*(E14/E11)</f>
         <v>0.71014088954534793</v>
       </c>
@@ -4295,7 +4324,7 @@
         <f t="shared" si="17"/>
         <v>na</v>
       </c>
-      <c r="BH14" s="75"/>
+      <c r="BH14" s="74"/>
     </row>
     <row r="15" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A15" s="21">
@@ -4439,41 +4468,41 @@
       <c r="AR15" s="23">
         <v>0</v>
       </c>
-      <c r="AS15" s="65">
+      <c r="AS15" s="64">
         <v>1</v>
       </c>
-      <c r="AT15" s="66">
+      <c r="AT15" s="65">
         <v>13</v>
       </c>
-      <c r="AU15" s="66">
+      <c r="AU15" s="65">
         <v>3</v>
       </c>
-      <c r="AV15" s="66">
+      <c r="AV15" s="65">
         <v>5</v>
       </c>
       <c r="AW15" s="35">
         <v>0</v>
       </c>
-      <c r="AX15" s="70">
+      <c r="AX15" s="69">
         <f t="shared" ref="AX15" si="18">AI15/AS15</f>
         <v>0</v>
       </c>
-      <c r="AY15" s="70">
+      <c r="AY15" s="69">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AZ15" s="70">
+      <c r="AZ15" s="69">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="BA15" s="69">
+      <c r="BA15" s="68">
         <f t="shared" si="13"/>
         <v>0.8</v>
       </c>
-      <c r="BB15" s="71" t="s">
+      <c r="BB15" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="BC15" s="78">
+      <c r="BC15" s="77">
         <v>1</v>
       </c>
       <c r="BD15" s="49">
@@ -4492,7 +4521,7 @@
         <f>BB15</f>
         <v>na</v>
       </c>
-      <c r="BH15" s="75"/>
+      <c r="BH15" s="74"/>
     </row>
     <row r="16" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A16" s="21">
@@ -4610,13 +4639,13 @@
       <c r="AJ16" s="47">
         <v>0</v>
       </c>
-      <c r="AK16" s="79">
+      <c r="AK16" s="78">
         <v>24</v>
       </c>
       <c r="AL16" s="47">
         <v>10</v>
       </c>
-      <c r="AM16" s="79">
+      <c r="AM16" s="78">
         <v>3</v>
       </c>
       <c r="AN16" s="47">
@@ -4634,37 +4663,37 @@
       <c r="AR16" s="23">
         <v>0</v>
       </c>
-      <c r="AS16" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT16" s="66">
+      <c r="AS16" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="65">
         <v>37</v>
       </c>
-      <c r="AU16" s="66">
+      <c r="AU16" s="65">
         <v>62</v>
       </c>
-      <c r="AV16" s="66">
+      <c r="AV16" s="65">
         <v>1</v>
       </c>
       <c r="AW16" s="35">
         <v>0</v>
       </c>
-      <c r="AX16" s="70" t="s">
+      <c r="AX16" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="AY16" s="70">
+      <c r="AY16" s="69">
         <f t="shared" si="15"/>
         <v>0.64864864864864868</v>
       </c>
-      <c r="AZ16" s="70">
+      <c r="AZ16" s="69">
         <f t="shared" si="12"/>
         <v>4.8387096774193547E-2</v>
       </c>
-      <c r="BA16" s="70">
+      <c r="BA16" s="69">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="BB16" s="71" t="s">
+      <c r="BB16" s="70" t="s">
         <v>67</v>
       </c>
       <c r="BC16" s="49" t="s">
@@ -4686,7 +4715,7 @@
         <f>BB16</f>
         <v>na</v>
       </c>
-      <c r="BH16" s="75"/>
+      <c r="BH16" s="74"/>
     </row>
     <row r="17" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A17" s="21">
@@ -4828,37 +4857,37 @@
       <c r="AR17" s="50">
         <v>0</v>
       </c>
-      <c r="AS17" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT17" s="66">
+      <c r="AS17" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="65">
         <v>29</v>
       </c>
-      <c r="AU17" s="66">
+      <c r="AU17" s="65">
         <v>166</v>
       </c>
-      <c r="AV17" s="66">
+      <c r="AV17" s="65">
         <v>26</v>
       </c>
       <c r="AW17" s="35">
         <v>0</v>
       </c>
-      <c r="AX17" s="69" t="s">
+      <c r="AX17" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="AY17" s="70">
+      <c r="AY17" s="69">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AZ17" s="70">
+      <c r="AZ17" s="69">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="BA17" s="70">
+      <c r="BA17" s="69">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="BB17" s="77" t="s">
+      <c r="BB17" s="76" t="s">
         <v>67</v>
       </c>
       <c r="BC17" s="32" t="str">
@@ -4877,10 +4906,10 @@
         <f>BF15*G17/G15</f>
         <v>0.55009905956112859</v>
       </c>
-      <c r="BG17" s="74" t="s">
+      <c r="BG17" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="BH17" s="75"/>
+      <c r="BH17" s="74"/>
     </row>
     <row r="18" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A18" s="21">
@@ -4896,7 +4925,7 @@
       <c r="D18" s="21">
         <v>184597</v>
       </c>
-      <c r="E18" s="76">
+      <c r="E18" s="75">
         <v>66794</v>
       </c>
       <c r="F18" s="44">
@@ -5023,37 +5052,37 @@
       <c r="AR18" s="52">
         <v>0</v>
       </c>
-      <c r="AS18" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT18" s="66">
+      <c r="AS18" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="65">
         <v>19</v>
       </c>
-      <c r="AU18" s="66">
+      <c r="AU18" s="65">
         <v>182</v>
       </c>
-      <c r="AV18" s="66">
+      <c r="AV18" s="65">
         <v>21</v>
       </c>
       <c r="AW18" s="35">
         <v>0</v>
       </c>
-      <c r="AX18" s="69" t="s">
+      <c r="AX18" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="AY18" s="69">
+      <c r="AY18" s="68">
         <f t="shared" si="15"/>
         <v>0.52631578947368418</v>
       </c>
-      <c r="AZ18" s="70">
+      <c r="AZ18" s="69">
         <f t="shared" si="12"/>
         <v>0.36263736263736263</v>
       </c>
-      <c r="BA18" s="70">
+      <c r="BA18" s="69">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="BB18" s="77" t="s">
+      <c r="BB18" s="76" t="s">
         <v>67</v>
       </c>
       <c r="BC18" s="32" t="str">
@@ -5072,10 +5101,10 @@
         <f>SUM(BF12*G12+BF15*G15)/SUM(G12,G15)</f>
         <v>0.84831751509922348</v>
       </c>
-      <c r="BG18" s="74" t="s">
+      <c r="BG18" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="BH18" s="75"/>
+      <c r="BH18" s="74"/>
     </row>
     <row r="19" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A19" s="21">
@@ -5091,7 +5120,7 @@
       <c r="D19" s="44">
         <v>422512</v>
       </c>
-      <c r="E19" s="76">
+      <c r="E19" s="75">
         <v>184597</v>
       </c>
       <c r="F19" s="21">
@@ -5186,7 +5215,7 @@
       <c r="AG19" s="32">
         <v>0.16825396825396827</v>
       </c>
-      <c r="AH19" s="80">
+      <c r="AH19" s="79">
         <v>3.1746031746031746E-3</v>
       </c>
       <c r="AI19" s="46">
@@ -5224,37 +5253,37 @@
       <c r="AR19" s="52">
         <v>1</v>
       </c>
-      <c r="AS19" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT19" s="66">
+      <c r="AS19" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="65">
         <v>134</v>
       </c>
-      <c r="AU19" s="66">
+      <c r="AU19" s="65">
         <v>127</v>
       </c>
-      <c r="AV19" s="66">
+      <c r="AV19" s="65">
         <v>52</v>
       </c>
       <c r="AW19" s="35">
         <v>1</v>
       </c>
-      <c r="AX19" s="70" t="s">
+      <c r="AX19" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="AY19" s="69">
+      <c r="AY19" s="68">
         <f t="shared" si="15"/>
         <v>0.61940298507462688</v>
       </c>
-      <c r="AZ19" s="69">
+      <c r="AZ19" s="68">
         <f t="shared" si="12"/>
         <v>0.52755905511811019</v>
       </c>
-      <c r="BA19" s="70">
+      <c r="BA19" s="69">
         <f t="shared" si="13"/>
         <v>0.21153846153846154</v>
       </c>
-      <c r="BB19" s="77">
+      <c r="BB19" s="76">
         <f t="shared" ref="BB19" si="19">AQ19/AW19</f>
         <v>0</v>
       </c>
@@ -5273,10 +5302,10 @@
         <f>BF15*G19/G15</f>
         <v>0.62670595611285274</v>
       </c>
-      <c r="BG19" s="74">
-        <v>0</v>
-      </c>
-      <c r="BH19" s="75"/>
+      <c r="BG19" s="73">
+        <v>0</v>
+      </c>
+      <c r="BH19" s="74"/>
     </row>
     <row r="20" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A20" s="21">
@@ -5362,10 +5391,10 @@
       </c>
       <c r="Y20" s="28"/>
       <c r="Z20" s="28">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="AA20" s="28">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="AB20" s="28">
         <v>13</v>
@@ -5386,23 +5415,23 @@
       <c r="AH20" s="26">
         <v>0</v>
       </c>
-      <c r="AI20" s="33">
-        <v>0</v>
-      </c>
-      <c r="AJ20" s="34">
+      <c r="AI20" s="46">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="47">
         <v>0</v>
       </c>
       <c r="AK20" s="46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL20" s="47">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AM20" s="33">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="AN20" s="34">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AO20" s="33">
         <v>0</v>
@@ -5416,40 +5445,40 @@
       <c r="AR20" s="52">
         <v>0</v>
       </c>
-      <c r="AS20" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT20" s="66">
-        <v>42</v>
-      </c>
-      <c r="AU20" s="66">
-        <v>129</v>
-      </c>
-      <c r="AV20" s="66">
+      <c r="AS20" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="65">
+        <v>49</v>
+      </c>
+      <c r="AU20" s="65">
+        <v>144</v>
+      </c>
+      <c r="AV20" s="65">
         <v>2</v>
       </c>
       <c r="AW20" s="35">
         <v>0</v>
       </c>
-      <c r="AX20" s="40" t="s">
+      <c r="AX20" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="AY20" s="70">
+      <c r="AY20" s="69">
         <f t="shared" si="15"/>
-        <v>4.7619047619047616E-2</v>
-      </c>
-      <c r="AZ20" s="69">
+        <v>2.0408163265306121E-2</v>
+      </c>
+      <c r="AZ20" s="68">
         <f t="shared" ref="AZ20" si="20">AM20/AU20</f>
-        <v>0.94573643410852715</v>
-      </c>
-      <c r="BA20" s="69">
+        <v>0.9375</v>
+      </c>
+      <c r="BA20" s="68">
         <f t="shared" ref="BA20" si="21">AO20/AV20</f>
         <v>0</v>
       </c>
-      <c r="BB20" s="77" t="s">
+      <c r="BB20" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="BC20" s="32" t="s">
+      <c r="BC20" s="49" t="s">
         <v>67</v>
       </c>
       <c r="BD20" s="49">
@@ -5458,16 +5487,16 @@
       </c>
       <c r="BE20" s="32">
         <f>AZ20</f>
-        <v>0.94573643410852715</v>
+        <v>0.9375</v>
       </c>
       <c r="BF20" s="32">
         <f>BF16*G20/G16</f>
         <v>0.16750846394984323</v>
       </c>
-      <c r="BG20" s="74" t="s">
+      <c r="BG20" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="BH20" s="75"/>
+      <c r="BH20" s="74"/>
     </row>
     <row r="21" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A21" s="21">
@@ -5546,22 +5575,22 @@
       <c r="AH21" s="26"/>
       <c r="AI21" s="33"/>
       <c r="AJ21" s="34"/>
-      <c r="AK21" s="33"/>
-      <c r="AL21" s="34"/>
+      <c r="AK21" s="46"/>
+      <c r="AL21" s="47"/>
       <c r="AM21" s="46"/>
       <c r="AN21" s="47"/>
       <c r="AO21" s="33"/>
       <c r="AP21" s="34"/>
       <c r="AQ21" s="33"/>
       <c r="AR21" s="35"/>
-      <c r="AS21" s="65"/>
-      <c r="AT21" s="66"/>
-      <c r="AU21" s="66"/>
-      <c r="AV21" s="66"/>
+      <c r="AS21" s="64"/>
+      <c r="AT21" s="65"/>
+      <c r="AU21" s="65"/>
+      <c r="AV21" s="65"/>
       <c r="AW21" s="35"/>
       <c r="AX21" s="21"/>
-      <c r="AY21" s="21"/>
-      <c r="AZ21" s="54"/>
+      <c r="AY21" s="53"/>
+      <c r="AZ21" s="53"/>
       <c r="BB21" s="36"/>
       <c r="BC21" s="32"/>
       <c r="BD21" s="32"/>
@@ -5590,7 +5619,7 @@
       </c>
       <c r="I22" s="24"/>
       <c r="J22" s="25"/>
-      <c r="K22" s="55"/>
+      <c r="K22" s="54"/>
       <c r="L22" s="25"/>
       <c r="M22" s="23"/>
       <c r="N22" s="27"/>
@@ -5626,20 +5655,21 @@
       <c r="AJ22" s="34"/>
       <c r="AK22" s="33"/>
       <c r="AL22" s="34"/>
-      <c r="AM22" s="33"/>
-      <c r="AN22" s="34"/>
+      <c r="AM22" s="46"/>
+      <c r="AN22" s="47"/>
       <c r="AO22" s="46"/>
       <c r="AP22" s="47"/>
       <c r="AQ22" s="33"/>
       <c r="AR22" s="35"/>
-      <c r="AS22" s="65"/>
-      <c r="AT22" s="66"/>
-      <c r="AU22" s="66"/>
-      <c r="AV22" s="66"/>
+      <c r="AS22" s="64"/>
+      <c r="AT22" s="65"/>
+      <c r="AU22" s="65"/>
+      <c r="AV22" s="65"/>
       <c r="AW22" s="35"/>
       <c r="AX22" s="21"/>
       <c r="AY22" s="21"/>
-      <c r="BA22" s="54"/>
+      <c r="AZ22" s="53"/>
+      <c r="BA22" s="53"/>
       <c r="BB22" s="36"/>
       <c r="BC22" s="32"/>
       <c r="BD22" s="32"/>
@@ -5702,18 +5732,19 @@
       <c r="AL23" s="34"/>
       <c r="AM23" s="33"/>
       <c r="AN23" s="34"/>
-      <c r="AO23" s="33"/>
-      <c r="AP23" s="34"/>
+      <c r="AO23" s="46"/>
+      <c r="AP23" s="47"/>
       <c r="AQ23" s="46"/>
       <c r="AR23" s="52"/>
-      <c r="AS23" s="65"/>
-      <c r="AT23" s="66"/>
-      <c r="AU23" s="66"/>
-      <c r="AV23" s="66"/>
+      <c r="AS23" s="64"/>
+      <c r="AT23" s="65"/>
+      <c r="AU23" s="65"/>
+      <c r="AV23" s="65"/>
       <c r="AW23" s="35"/>
       <c r="AX23" s="21"/>
       <c r="AY23" s="21"/>
-      <c r="BB23" s="56"/>
+      <c r="BA23" s="53"/>
+      <c r="BB23" s="55"/>
       <c r="BG23" s="36"/>
     </row>
     <row r="24" spans="1:60" x14ac:dyDescent="0.2">
@@ -5728,7 +5759,7 @@
       <c r="G24" s="21">
         <v>478224</v>
       </c>
-      <c r="H24" s="57">
+      <c r="H24" s="56">
         <v>500039</v>
       </c>
       <c r="I24" s="27"/>
@@ -5767,16 +5798,16 @@
       <c r="AN24" s="34"/>
       <c r="AO24" s="33"/>
       <c r="AP24" s="34"/>
-      <c r="AQ24" s="33"/>
-      <c r="AR24" s="35"/>
-      <c r="AS24" s="65"/>
-      <c r="AT24" s="66"/>
-      <c r="AU24" s="66"/>
-      <c r="AV24" s="66"/>
+      <c r="AQ24" s="46"/>
+      <c r="AR24" s="47"/>
+      <c r="AS24" s="64"/>
+      <c r="AT24" s="65"/>
+      <c r="AU24" s="65"/>
+      <c r="AV24" s="65"/>
       <c r="AW24" s="35"/>
       <c r="AX24" s="21"/>
       <c r="AY24" s="21"/>
-      <c r="BB24" s="36"/>
+      <c r="BB24" s="55"/>
       <c r="BG24" s="36"/>
     </row>
     <row r="25" spans="1:60" x14ac:dyDescent="0.2">
@@ -5817,19 +5848,19 @@
       <c r="AG25" s="21"/>
       <c r="AH25" s="23"/>
       <c r="AI25" s="21"/>
-      <c r="AJ25" s="58"/>
+      <c r="AJ25" s="57"/>
       <c r="AK25" s="21"/>
-      <c r="AL25" s="58"/>
+      <c r="AL25" s="57"/>
       <c r="AM25" s="21"/>
-      <c r="AN25" s="58"/>
+      <c r="AN25" s="57"/>
       <c r="AO25" s="21"/>
-      <c r="AP25" s="58"/>
+      <c r="AP25" s="57"/>
       <c r="AQ25" s="21"/>
       <c r="AR25" s="23"/>
       <c r="AS25" s="27"/>
       <c r="AT25" s="28"/>
-      <c r="AU25" s="59"/>
-      <c r="AV25" s="59"/>
+      <c r="AU25" s="58"/>
+      <c r="AV25" s="58"/>
       <c r="AW25" s="36"/>
       <c r="AX25" s="21"/>
       <c r="AY25" s="21"/>
@@ -5872,19 +5903,19 @@
       <c r="AG26" s="21"/>
       <c r="AH26" s="23"/>
       <c r="AI26" s="21"/>
-      <c r="AJ26" s="58"/>
+      <c r="AJ26" s="57"/>
       <c r="AK26" s="21"/>
-      <c r="AL26" s="58"/>
+      <c r="AL26" s="57"/>
       <c r="AM26" s="21"/>
-      <c r="AN26" s="58"/>
+      <c r="AN26" s="57"/>
       <c r="AO26" s="21"/>
-      <c r="AP26" s="58"/>
+      <c r="AP26" s="57"/>
       <c r="AQ26" s="21"/>
       <c r="AR26" s="23"/>
-      <c r="AS26" s="60"/>
-      <c r="AT26" s="59"/>
-      <c r="AU26" s="59"/>
-      <c r="AV26" s="59"/>
+      <c r="AS26" s="59"/>
+      <c r="AT26" s="58"/>
+      <c r="AU26" s="58"/>
+      <c r="AV26" s="58"/>
       <c r="AW26" s="36"/>
       <c r="BB26" s="36"/>
       <c r="BG26" s="36"/>
@@ -5918,19 +5949,19 @@
       <c r="AA27" s="28"/>
       <c r="AB27" s="28"/>
       <c r="AC27" s="23"/>
-      <c r="AD27" s="61"/>
-      <c r="AE27" s="61"/>
-      <c r="AF27" s="61"/>
-      <c r="AG27" s="61"/>
-      <c r="AH27" s="62"/>
+      <c r="AD27" s="60"/>
+      <c r="AE27" s="60"/>
+      <c r="AF27" s="60"/>
+      <c r="AG27" s="60"/>
+      <c r="AH27" s="61"/>
       <c r="AI27" s="21"/>
-      <c r="AJ27" s="58"/>
+      <c r="AJ27" s="57"/>
       <c r="AK27" s="21"/>
-      <c r="AL27" s="58"/>
+      <c r="AL27" s="57"/>
       <c r="AM27" s="21"/>
-      <c r="AN27" s="58"/>
+      <c r="AN27" s="57"/>
       <c r="AO27" s="21"/>
-      <c r="AP27" s="58"/>
+      <c r="AP27" s="57"/>
       <c r="AQ27" s="21"/>
       <c r="AR27" s="23"/>
       <c r="AW27" s="36"/>
@@ -5938,197 +5969,197 @@
       <c r="BG27" s="36"/>
     </row>
     <row r="28" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="C28" s="63"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
       <c r="H28" s="36"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
       <c r="M28" s="36"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="58"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="58"/>
       <c r="R28" s="36"/>
-      <c r="S28" s="60"/>
-      <c r="T28" s="59"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="59"/>
+      <c r="S28" s="59"/>
+      <c r="T28" s="58"/>
+      <c r="U28" s="58"/>
+      <c r="V28" s="58"/>
       <c r="W28" s="36"/>
       <c r="X28" s="36"/>
-      <c r="Y28" s="60"/>
-      <c r="Z28" s="59"/>
-      <c r="AA28" s="59"/>
-      <c r="AB28" s="59"/>
+      <c r="Y28" s="59"/>
+      <c r="Z28" s="58"/>
+      <c r="AA28" s="58"/>
+      <c r="AB28" s="58"/>
       <c r="AC28" s="36"/>
       <c r="AH28" s="36"/>
-      <c r="AJ28" s="64"/>
-      <c r="AL28" s="64"/>
-      <c r="AN28" s="64"/>
-      <c r="AP28" s="64"/>
+      <c r="AJ28" s="63"/>
+      <c r="AL28" s="63"/>
+      <c r="AN28" s="63"/>
+      <c r="AP28" s="63"/>
       <c r="AR28" s="36"/>
       <c r="AW28" s="36"/>
       <c r="BB28" s="36"/>
       <c r="BG28" s="36"/>
     </row>
     <row r="29" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="C29" s="63"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
       <c r="H29" s="36"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="59"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
       <c r="M29" s="36"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="58"/>
+      <c r="P29" s="58"/>
+      <c r="Q29" s="58"/>
       <c r="R29" s="36"/>
-      <c r="S29" s="60"/>
-      <c r="T29" s="59"/>
-      <c r="U29" s="59"/>
-      <c r="V29" s="59"/>
+      <c r="S29" s="59"/>
+      <c r="T29" s="58"/>
+      <c r="U29" s="58"/>
+      <c r="V29" s="58"/>
       <c r="W29" s="36"/>
       <c r="X29" s="36"/>
-      <c r="Y29" s="60"/>
-      <c r="Z29" s="59"/>
-      <c r="AA29" s="59"/>
-      <c r="AB29" s="59"/>
+      <c r="Y29" s="59"/>
+      <c r="Z29" s="58"/>
+      <c r="AA29" s="58"/>
+      <c r="AB29" s="58"/>
       <c r="AC29" s="36"/>
       <c r="AH29" s="36"/>
-      <c r="AJ29" s="64"/>
-      <c r="AL29" s="64"/>
-      <c r="AN29" s="64"/>
-      <c r="AP29" s="64"/>
+      <c r="AJ29" s="63"/>
+      <c r="AL29" s="63"/>
+      <c r="AN29" s="63"/>
+      <c r="AP29" s="63"/>
       <c r="AR29" s="36"/>
       <c r="AW29" s="36"/>
       <c r="BB29" s="36"/>
       <c r="BG29" s="36"/>
     </row>
     <row r="30" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="C30" s="63"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
       <c r="H30" s="36"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="59"/>
-      <c r="K30" s="59"/>
-      <c r="L30" s="59"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
       <c r="M30" s="36"/>
-      <c r="N30" s="60"/>
-      <c r="O30" s="59"/>
-      <c r="P30" s="59"/>
-      <c r="Q30" s="59"/>
+      <c r="N30" s="59"/>
+      <c r="O30" s="58"/>
+      <c r="P30" s="58"/>
+      <c r="Q30" s="58"/>
       <c r="R30" s="36"/>
-      <c r="S30" s="60"/>
-      <c r="T30" s="59"/>
-      <c r="U30" s="59"/>
-      <c r="V30" s="59"/>
+      <c r="S30" s="59"/>
+      <c r="T30" s="58"/>
+      <c r="U30" s="58"/>
+      <c r="V30" s="58"/>
       <c r="W30" s="36"/>
       <c r="X30" s="36"/>
-      <c r="Y30" s="60"/>
-      <c r="Z30" s="59"/>
-      <c r="AA30" s="59"/>
-      <c r="AB30" s="59"/>
+      <c r="Y30" s="59"/>
+      <c r="Z30" s="58"/>
+      <c r="AA30" s="58"/>
+      <c r="AB30" s="58"/>
       <c r="AC30" s="36"/>
       <c r="AH30" s="36"/>
-      <c r="AJ30" s="64"/>
-      <c r="AL30" s="64"/>
-      <c r="AN30" s="64"/>
-      <c r="AP30" s="64"/>
+      <c r="AJ30" s="63"/>
+      <c r="AL30" s="63"/>
+      <c r="AN30" s="63"/>
+      <c r="AP30" s="63"/>
       <c r="AR30" s="36"/>
       <c r="AW30" s="36"/>
       <c r="BB30" s="36"/>
       <c r="BG30" s="36"/>
     </row>
     <row r="31" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="C31" s="63"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
       <c r="H31" s="36"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="59"/>
-      <c r="L31" s="59"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
       <c r="M31" s="36"/>
-      <c r="N31" s="60"/>
-      <c r="O31" s="59"/>
-      <c r="P31" s="59"/>
-      <c r="Q31" s="59"/>
+      <c r="N31" s="59"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="58"/>
       <c r="R31" s="36"/>
-      <c r="S31" s="60"/>
-      <c r="T31" s="59"/>
-      <c r="U31" s="59"/>
-      <c r="V31" s="59"/>
+      <c r="S31" s="59"/>
+      <c r="T31" s="58"/>
+      <c r="U31" s="58"/>
+      <c r="V31" s="58"/>
       <c r="W31" s="36"/>
       <c r="X31" s="36"/>
-      <c r="Y31" s="60"/>
-      <c r="Z31" s="59"/>
-      <c r="AA31" s="59"/>
-      <c r="AB31" s="59"/>
+      <c r="Y31" s="59"/>
+      <c r="Z31" s="58"/>
+      <c r="AA31" s="58"/>
+      <c r="AB31" s="58"/>
       <c r="AC31" s="36"/>
       <c r="AH31" s="36"/>
-      <c r="AJ31" s="64"/>
-      <c r="AL31" s="64"/>
-      <c r="AN31" s="64"/>
-      <c r="AP31" s="64"/>
+      <c r="AJ31" s="63"/>
+      <c r="AL31" s="63"/>
+      <c r="AN31" s="63"/>
+      <c r="AP31" s="63"/>
       <c r="AR31" s="36"/>
       <c r="AW31" s="36"/>
       <c r="BB31" s="36"/>
       <c r="BG31" s="36"/>
     </row>
     <row r="32" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="C32" s="63"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
       <c r="H32" s="36"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="59"/>
-      <c r="K32" s="59"/>
-      <c r="L32" s="59"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
       <c r="M32" s="36"/>
-      <c r="N32" s="60"/>
-      <c r="O32" s="59"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="59"/>
+      <c r="N32" s="59"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="58"/>
+      <c r="Q32" s="58"/>
       <c r="R32" s="36"/>
-      <c r="S32" s="60"/>
-      <c r="T32" s="59"/>
-      <c r="U32" s="59"/>
-      <c r="V32" s="59"/>
+      <c r="S32" s="59"/>
+      <c r="T32" s="58"/>
+      <c r="U32" s="58"/>
+      <c r="V32" s="58"/>
       <c r="W32" s="36"/>
       <c r="X32" s="36"/>
-      <c r="Y32" s="60"/>
-      <c r="Z32" s="59"/>
-      <c r="AA32" s="59"/>
-      <c r="AB32" s="59"/>
+      <c r="Y32" s="59"/>
+      <c r="Z32" s="58"/>
+      <c r="AA32" s="58"/>
+      <c r="AB32" s="58"/>
       <c r="AC32" s="36"/>
       <c r="AH32" s="36"/>
-      <c r="AJ32" s="64"/>
-      <c r="AL32" s="64"/>
-      <c r="AN32" s="64"/>
-      <c r="AP32" s="64"/>
+      <c r="AJ32" s="63"/>
+      <c r="AL32" s="63"/>
+      <c r="AN32" s="63"/>
+      <c r="AP32" s="63"/>
       <c r="AR32" s="36"/>
       <c r="AW32" s="36"/>
       <c r="BB32" s="36"/>
       <c r="BG32" s="36"/>
     </row>
     <row r="33" spans="42:42" x14ac:dyDescent="0.2">
-      <c r="AP33" s="64"/>
+      <c r="AP33" s="63"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -6211,8 +6242,8 @@
   <dimension ref="A1:BQ25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R40" sqref="R40"/>
+      <pane xSplit="1" topLeftCell="AS1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AZ28" sqref="AZ28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6234,62 +6265,62 @@
       <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="BK1" s="64"/>
+      <c r="BK1" s="63"/>
     </row>
     <row r="2" spans="1:69" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="BK2" s="64"/>
-      <c r="BM2" s="64"/>
+      <c r="BK2" s="63"/>
+      <c r="BM2" s="63"/>
     </row>
     <row r="3" spans="1:69" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B3" s="36"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
       <c r="H3" s="36"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="82" t="s">
+      <c r="I3" s="58"/>
+      <c r="J3" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
       <c r="M3" s="36"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="36"/>
-      <c r="S3" s="60"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="59"/>
-      <c r="V3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
       <c r="W3" s="36"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="59" t="s">
+      <c r="X3" s="62"/>
+      <c r="Y3" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="Z3" s="59"/>
-      <c r="AA3" s="59"/>
-      <c r="AB3" s="59"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58"/>
       <c r="AC3" s="36"/>
-      <c r="AD3" s="60" t="s">
+      <c r="AD3" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="AI3" s="60" t="s">
+      <c r="AI3" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="AJ3" s="59"/>
-      <c r="AK3" s="59"/>
-      <c r="AL3" s="59"/>
-      <c r="AM3" s="59"/>
-      <c r="AN3" s="59"/>
-      <c r="AO3" s="59"/>
-      <c r="AP3" s="59"/>
-      <c r="AQ3" s="59"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58"/>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="58"/>
+      <c r="AN3" s="58"/>
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58"/>
       <c r="AR3" s="36"/>
-      <c r="AS3" s="59" t="s">
-        <v>78</v>
+      <c r="AS3" s="58" t="s">
+        <v>86</v>
       </c>
       <c r="AZ3" s="11" t="s">
         <v>63</v>
@@ -6297,17 +6328,17 @@
       <c r="BE3" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="BH3" s="60" t="s">
+      <c r="BH3" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="BI3" s="59"/>
-      <c r="BJ3" s="59"/>
-      <c r="BK3" s="64"/>
-      <c r="BL3" s="59"/>
-      <c r="BM3" s="64"/>
-      <c r="BN3" s="59"/>
-      <c r="BO3" s="64"/>
-      <c r="BP3" s="59"/>
+      <c r="BI3" s="58"/>
+      <c r="BJ3" s="58"/>
+      <c r="BK3" s="63"/>
+      <c r="BL3" s="58"/>
+      <c r="BM3" s="63"/>
+      <c r="BN3" s="58"/>
+      <c r="BO3" s="63"/>
+      <c r="BP3" s="58"/>
       <c r="BQ3" s="36"/>
     </row>
     <row r="4" spans="1:69" s="13" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -6863,10 +6894,10 @@
       <c r="AP7" s="34"/>
       <c r="AQ7" s="33"/>
       <c r="AR7" s="35"/>
-      <c r="AS7" s="65"/>
-      <c r="AT7" s="66"/>
-      <c r="AU7" s="66"/>
-      <c r="AV7" s="66"/>
+      <c r="AS7" s="64"/>
+      <c r="AT7" s="65"/>
+      <c r="AU7" s="65"/>
+      <c r="AV7" s="65"/>
       <c r="AW7" s="35"/>
       <c r="AX7" s="40"/>
       <c r="AY7" s="41"/>
@@ -6987,10 +7018,10 @@
       <c r="AP8" s="34"/>
       <c r="AQ8" s="33"/>
       <c r="AR8" s="35"/>
-      <c r="AS8" s="65"/>
-      <c r="AT8" s="66"/>
-      <c r="AU8" s="66"/>
-      <c r="AV8" s="66"/>
+      <c r="AS8" s="64"/>
+      <c r="AT8" s="65"/>
+      <c r="AU8" s="65"/>
+      <c r="AV8" s="65"/>
       <c r="AW8" s="35"/>
       <c r="AX8" s="44"/>
       <c r="AY8" s="41"/>
@@ -7130,13 +7161,13 @@
       <c r="AI9" s="33">
         <v>0</v>
       </c>
-      <c r="AJ9" s="67">
+      <c r="AJ9" s="66">
         <v>3</v>
       </c>
       <c r="AK9" s="46">
         <v>0</v>
       </c>
-      <c r="AL9" s="68">
+      <c r="AL9" s="67">
         <v>10</v>
       </c>
       <c r="AM9" s="33">
@@ -7157,50 +7188,50 @@
       <c r="AR9" s="35">
         <v>1</v>
       </c>
-      <c r="AS9" s="65">
+      <c r="AS9" s="64">
         <v>3</v>
       </c>
-      <c r="AT9" s="66">
+      <c r="AT9" s="65">
         <v>10</v>
       </c>
-      <c r="AU9" s="66">
+      <c r="AU9" s="65">
         <v>33</v>
       </c>
-      <c r="AV9" s="66">
+      <c r="AV9" s="65">
         <v>38</v>
       </c>
       <c r="AW9" s="35">
         <v>1</v>
       </c>
-      <c r="AX9" s="69">
+      <c r="AX9" s="68">
         <f>AI9/SUM(AI9:AJ9)</f>
         <v>0</v>
       </c>
-      <c r="AY9" s="70">
+      <c r="AY9" s="69">
         <f>AK9/SUM(AK9:AL9)</f>
         <v>0</v>
       </c>
-      <c r="AZ9" s="69">
+      <c r="AZ9" s="68">
         <f>AM9/SUM(AM9:AN9)</f>
         <v>0</v>
       </c>
-      <c r="BA9" s="69">
+      <c r="BA9" s="68">
         <f>AO9/SUM(AO9:AP9)</f>
         <v>0</v>
       </c>
-      <c r="BB9" s="71">
+      <c r="BB9" s="70">
         <f>AQ9/SUM(AQ9:AR9)</f>
         <v>0</v>
       </c>
-      <c r="BC9" s="72">
+      <c r="BC9" s="71">
         <f>AX9</f>
         <v>0</v>
       </c>
-      <c r="BD9" s="73">
+      <c r="BD9" s="72">
         <f>(SUM(BD11*E11+BD12*E12)/SUM(E11:E12))*(E9/E12)</f>
         <v>0.91671796261049654</v>
       </c>
-      <c r="BE9" s="73">
+      <c r="BE9" s="72">
         <f>AVERAGE(BE11,BE17)</f>
         <v>0.94495111833035983</v>
       </c>
@@ -7208,47 +7239,47 @@
         <f>SUM(BF12*G12+BF15*G15)/SUM(G12,G15)</f>
         <v>0.84831751509922348</v>
       </c>
-      <c r="BG9" s="74">
+      <c r="BG9" s="73">
         <f>BB9</f>
         <v>0</v>
       </c>
-      <c r="BH9" s="83">
+      <c r="BH9" s="82">
         <f>SUM(AI9:AJ9)*BC9</f>
         <v>0</v>
       </c>
-      <c r="BI9" s="67">
+      <c r="BI9" s="66">
         <f>SUM(AI9:AJ9)-BH9</f>
         <v>3</v>
       </c>
-      <c r="BJ9" s="83">
+      <c r="BJ9" s="82">
         <f>SUM(AK9:AL9)*BD9</f>
         <v>9.1671796261049661</v>
       </c>
-      <c r="BK9" s="84">
+      <c r="BK9" s="83">
         <f>SUM(AK9:AL9)-BJ9</f>
         <v>0.83282037389503394</v>
       </c>
-      <c r="BL9" s="91">
+      <c r="BL9" s="90">
         <f>SUM(AM9:AN9)*BE9</f>
         <v>29.293484668241156</v>
       </c>
-      <c r="BM9" s="93">
+      <c r="BM9" s="92">
         <f>SUM(AM9:AN9)-BL9</f>
         <v>1.706515331758844</v>
       </c>
-      <c r="BN9" s="91">
+      <c r="BN9" s="90">
         <f>SUM(AO9:AP9)*BF9</f>
         <v>32.236065573770489</v>
       </c>
-      <c r="BO9" s="93">
+      <c r="BO9" s="92">
         <f>SUM(AO9:AP9)-BN9</f>
         <v>5.7639344262295111</v>
       </c>
-      <c r="BP9" s="91">
+      <c r="BP9" s="90">
         <f>SUM(AQ9:AR9)*BG9</f>
         <v>0</v>
       </c>
-      <c r="BQ9" s="92">
+      <c r="BQ9" s="91">
         <f>SUM(AQ9:AR9)-BP9</f>
         <v>1</v>
       </c>
@@ -7377,34 +7408,34 @@
       <c r="AR10" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AS10" s="65" t="s">
-        <v>57</v>
-      </c>
-      <c r="AT10" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="AU10" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV10" s="66" t="s">
+      <c r="AS10" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT10" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU10" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV10" s="65" t="s">
         <v>57</v>
       </c>
       <c r="AW10" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AX10" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="AY10" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="AZ10" s="70" t="s">
-        <v>57</v>
-      </c>
-      <c r="BA10" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="BB10" s="71" t="s">
+      <c r="AX10" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY10" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ10" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA10" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB10" s="70" t="s">
         <v>57</v>
       </c>
       <c r="BC10" s="32" t="s">
@@ -7425,7 +7456,7 @@
       <c r="BH10" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="BI10" s="67" t="s">
+      <c r="BI10" s="66" t="s">
         <v>57</v>
       </c>
       <c r="BJ10" s="33" t="s">
@@ -7434,10 +7465,10 @@
       <c r="BK10" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="BL10" s="83" t="s">
-        <v>57</v>
-      </c>
-      <c r="BM10" s="84" t="s">
+      <c r="BL10" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="BM10" s="83" t="s">
         <v>57</v>
       </c>
       <c r="BN10" s="33" t="s">
@@ -7467,7 +7498,7 @@
       <c r="D11" s="21">
         <v>1031800</v>
       </c>
-      <c r="E11" s="76">
+      <c r="E11" s="75">
         <v>245000</v>
       </c>
       <c r="F11" s="21">
@@ -7593,37 +7624,37 @@
       <c r="AR11" s="35">
         <v>0</v>
       </c>
-      <c r="AS11" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="66">
+      <c r="AS11" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="65">
         <v>11</v>
       </c>
-      <c r="AU11" s="66">
+      <c r="AU11" s="65">
         <v>85</v>
       </c>
-      <c r="AV11" s="66">
+      <c r="AV11" s="65">
         <v>7</v>
       </c>
       <c r="AW11" s="35">
         <v>0</v>
       </c>
-      <c r="AX11" s="69" t="s">
+      <c r="AX11" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="AY11" s="69">
+      <c r="AY11" s="68">
         <f>AK11/SUM(AK11:AL11)</f>
         <v>0.9</v>
       </c>
-      <c r="AZ11" s="69">
+      <c r="AZ11" s="68">
         <f>AM11/SUM(AM11:AN11)</f>
         <v>0.97530864197530864</v>
       </c>
-      <c r="BA11" s="70">
+      <c r="BA11" s="69">
         <f>AO11/AV11</f>
         <v>0</v>
       </c>
-      <c r="BB11" s="71" t="s">
+      <c r="BB11" s="70" t="s">
         <v>67</v>
       </c>
       <c r="BC11" s="32" t="str">
@@ -7649,7 +7680,7 @@
       <c r="BH11" s="33">
         <v>0</v>
       </c>
-      <c r="BI11" s="67">
+      <c r="BI11" s="66">
         <v>0</v>
       </c>
       <c r="BJ11" s="33">
@@ -7666,11 +7697,11 @@
       <c r="BM11" s="34">
         <v>2</v>
       </c>
-      <c r="BN11" s="83">
+      <c r="BN11" s="82">
         <f>SUM(AO11:AP11)*BF11</f>
         <v>4.0389970660737253</v>
       </c>
-      <c r="BO11" s="84">
+      <c r="BO11" s="83">
         <f>SUM(AO11:AP11)-BN11</f>
         <v>0.96100293392627467</v>
       </c>
@@ -7695,7 +7726,7 @@
       <c r="D12" s="21">
         <v>319000</v>
       </c>
-      <c r="E12" s="76">
+      <c r="E12" s="75">
         <v>1031800</v>
       </c>
       <c r="F12" s="21">
@@ -7821,37 +7852,37 @@
       <c r="AR12" s="52">
         <v>0</v>
       </c>
-      <c r="AS12" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT12" s="66">
+      <c r="AS12" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="65">
         <v>23</v>
       </c>
-      <c r="AU12" s="66">
+      <c r="AU12" s="65">
         <v>36</v>
       </c>
-      <c r="AV12" s="66">
+      <c r="AV12" s="65">
         <v>30</v>
       </c>
       <c r="AW12" s="35">
         <v>0</v>
       </c>
-      <c r="AX12" s="69" t="s">
+      <c r="AX12" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="AY12" s="69">
+      <c r="AY12" s="68">
         <f>AK12/SUM(AK12:AL12)</f>
         <v>0.91304347826086951</v>
       </c>
-      <c r="AZ12" s="69">
+      <c r="AZ12" s="68">
         <f>AM12/SUM(AM12:AN12)</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="BA12" s="69">
+      <c r="BA12" s="68">
         <f>AO12/SUM(AO12:AP12)</f>
         <v>0.8666666666666667</v>
       </c>
-      <c r="BB12" s="77" t="s">
+      <c r="BB12" s="76" t="s">
         <v>67</v>
       </c>
       <c r="BC12" s="32" t="str">
@@ -7870,13 +7901,13 @@
         <f t="shared" si="11"/>
         <v>0.8666666666666667</v>
       </c>
-      <c r="BG12" s="74" t="s">
+      <c r="BG12" s="73" t="s">
         <v>67</v>
       </c>
       <c r="BH12" s="33">
         <v>0</v>
       </c>
-      <c r="BI12" s="67">
+      <c r="BI12" s="66">
         <v>0</v>
       </c>
       <c r="BJ12" s="33">
@@ -7901,10 +7932,10 @@
         <f>AP12</f>
         <v>4</v>
       </c>
-      <c r="BP12" s="83">
-        <v>0</v>
-      </c>
-      <c r="BQ12" s="85">
+      <c r="BP12" s="82">
+        <v>0</v>
+      </c>
+      <c r="BQ12" s="84">
         <v>0</v>
       </c>
     </row>
@@ -8032,34 +8063,34 @@
       <c r="AR13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AS13" s="65" t="s">
-        <v>57</v>
-      </c>
-      <c r="AT13" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="AU13" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV13" s="66" t="s">
+      <c r="AS13" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT13" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU13" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV13" s="65" t="s">
         <v>57</v>
       </c>
       <c r="AW13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AX13" s="70" t="s">
-        <v>57</v>
-      </c>
-      <c r="AY13" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="AZ13" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="BA13" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="BB13" s="71" t="s">
+      <c r="AX13" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY13" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ13" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA13" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB13" s="70" t="s">
         <v>57</v>
       </c>
       <c r="BC13" s="49" t="s">
@@ -8077,10 +8108,10 @@
       <c r="BG13" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="BH13" s="83" t="s">
-        <v>57</v>
-      </c>
-      <c r="BI13" s="84" t="s">
+      <c r="BH13" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI13" s="83" t="s">
         <v>57</v>
       </c>
       <c r="BJ13" s="33" t="s">
@@ -8252,43 +8283,43 @@
       <c r="AR14" s="35">
         <v>0</v>
       </c>
-      <c r="AS14" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT14" s="66">
+      <c r="AS14" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="65">
         <v>25</v>
       </c>
-      <c r="AU14" s="66">
+      <c r="AU14" s="65">
         <v>53</v>
       </c>
-      <c r="AV14" s="66">
+      <c r="AV14" s="65">
         <v>15</v>
       </c>
       <c r="AW14" s="35">
         <v>1</v>
       </c>
-      <c r="AX14" s="70" t="s">
+      <c r="AX14" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="AY14" s="70">
+      <c r="AY14" s="69">
         <f>AK14/SUM(AK14:AL14)</f>
         <v>0.13636363636363635</v>
       </c>
-      <c r="AZ14" s="69">
+      <c r="AZ14" s="68">
         <f>AM14/SUM(AM14:AN14)</f>
         <v>0.75471698113207553</v>
       </c>
-      <c r="BA14" s="69">
+      <c r="BA14" s="68">
         <f t="shared" ref="BA14:BA15" si="13">AO14/SUM(AO14:AP14)</f>
         <v>0.75</v>
       </c>
-      <c r="BB14" s="71" t="s">
+      <c r="BB14" s="70" t="s">
         <v>67</v>
       </c>
       <c r="BC14" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="BD14" s="73">
+      <c r="BD14" s="72">
         <f>SUM(BD11*E11+BD19*E19)/SUM(E11,E19)*(E14/E11)</f>
         <v>0.77393271419094112</v>
       </c>
@@ -8304,17 +8335,17 @@
         <f t="shared" si="14"/>
         <v>na</v>
       </c>
-      <c r="BH14" s="83">
-        <v>0</v>
-      </c>
-      <c r="BI14" s="84">
-        <v>0</v>
-      </c>
-      <c r="BJ14" s="83">
+      <c r="BH14" s="82">
+        <v>0</v>
+      </c>
+      <c r="BI14" s="83">
+        <v>0</v>
+      </c>
+      <c r="BJ14" s="82">
         <f>SUM(AK14:AL14)*BD14</f>
         <v>17.026519712200706</v>
       </c>
-      <c r="BK14" s="84">
+      <c r="BK14" s="83">
         <f>SUM(AK14:AL14)-BJ14</f>
         <v>4.9734802877992941</v>
       </c>
@@ -8481,41 +8512,41 @@
       <c r="AR15" s="23">
         <v>0</v>
       </c>
-      <c r="AS15" s="65">
+      <c r="AS15" s="64">
         <v>1</v>
       </c>
-      <c r="AT15" s="66">
+      <c r="AT15" s="65">
         <v>13</v>
       </c>
-      <c r="AU15" s="66">
+      <c r="AU15" s="65">
         <v>3</v>
       </c>
-      <c r="AV15" s="66">
+      <c r="AV15" s="65">
         <v>5</v>
       </c>
       <c r="AW15" s="35">
         <v>0</v>
       </c>
-      <c r="AX15" s="70">
+      <c r="AX15" s="69">
         <f>AI15/SUM(AI15:AJ15)</f>
         <v>0</v>
       </c>
-      <c r="AY15" s="70">
+      <c r="AY15" s="69">
         <f t="shared" ref="AY15:AY17" si="15">AK15/SUM(AK15:AL15)</f>
         <v>0</v>
       </c>
-      <c r="AZ15" s="70">
+      <c r="AZ15" s="69">
         <f>AM15/SUM(AM15:AN15)</f>
         <v>0</v>
       </c>
-      <c r="BA15" s="69">
+      <c r="BA15" s="68">
         <f t="shared" si="13"/>
         <v>0.8</v>
       </c>
-      <c r="BB15" s="71" t="s">
+      <c r="BB15" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="BC15" s="78">
+      <c r="BC15" s="77">
         <v>1</v>
       </c>
       <c r="BD15" s="49">
@@ -8534,27 +8565,27 @@
         <f>BB15</f>
         <v>na</v>
       </c>
-      <c r="BH15" s="83">
+      <c r="BH15" s="82">
         <f>SUM(AI15:AJ15)*BC15</f>
         <v>1</v>
       </c>
-      <c r="BI15" s="84">
+      <c r="BI15" s="83">
         <f>SUM(AI15:AJ15)-BH15</f>
         <v>0</v>
       </c>
-      <c r="BJ15" s="83">
+      <c r="BJ15" s="82">
         <f>SUM(AK15:AL15)*BD15</f>
         <v>9.2948720845778716</v>
       </c>
-      <c r="BK15" s="84">
+      <c r="BK15" s="83">
         <f>SUM(AK15:AL15)-BJ15</f>
         <v>3.7051279154221284</v>
       </c>
-      <c r="BL15" s="83">
+      <c r="BL15" s="82">
         <f>SUM(AM15:AN15)*BE15</f>
         <v>2.2068550111734782</v>
       </c>
-      <c r="BM15" s="84">
+      <c r="BM15" s="83">
         <f>SUM(AM15:AN15)-BL15</f>
         <v>0.79314498882652185</v>
       </c>
@@ -8689,13 +8720,13 @@
       <c r="AJ16" s="47">
         <v>0</v>
       </c>
-      <c r="AK16" s="79">
+      <c r="AK16" s="78">
         <v>24</v>
       </c>
       <c r="AL16" s="47">
         <v>10</v>
       </c>
-      <c r="AM16" s="79">
+      <c r="AM16" s="78">
         <v>3</v>
       </c>
       <c r="AN16" s="47">
@@ -8713,37 +8744,37 @@
       <c r="AR16" s="23">
         <v>0</v>
       </c>
-      <c r="AS16" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT16" s="66">
+      <c r="AS16" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="65">
         <v>37</v>
       </c>
-      <c r="AU16" s="66">
+      <c r="AU16" s="65">
         <v>62</v>
       </c>
-      <c r="AV16" s="66">
+      <c r="AV16" s="65">
         <v>1</v>
       </c>
       <c r="AW16" s="35">
         <v>0</v>
       </c>
-      <c r="AX16" s="70" t="s">
+      <c r="AX16" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="AY16" s="70">
+      <c r="AY16" s="69">
         <f t="shared" si="15"/>
         <v>0.70588235294117652</v>
       </c>
-      <c r="AZ16" s="70">
+      <c r="AZ16" s="69">
         <f t="shared" ref="AZ16:AZ18" si="16">AM16/SUM(AM16:AN16)</f>
         <v>4.9180327868852458E-2</v>
       </c>
-      <c r="BA16" s="70">
+      <c r="BA16" s="69">
         <f>AO16/SUM(AO16:AP16)</f>
         <v>0</v>
       </c>
-      <c r="BB16" s="71" t="s">
+      <c r="BB16" s="70" t="s">
         <v>67</v>
       </c>
       <c r="BC16" s="49" t="s">
@@ -8765,33 +8796,33 @@
         <f>BB16</f>
         <v>na</v>
       </c>
-      <c r="BH16" s="83">
-        <v>0</v>
-      </c>
-      <c r="BI16" s="84">
-        <v>0</v>
-      </c>
-      <c r="BJ16" s="83">
+      <c r="BH16" s="82">
+        <v>0</v>
+      </c>
+      <c r="BI16" s="83">
+        <v>0</v>
+      </c>
+      <c r="BJ16" s="82">
         <f>AK16+(AL16*BD16)</f>
         <v>33.105406178489702</v>
       </c>
-      <c r="BK16" s="84">
+      <c r="BK16" s="83">
         <f>SUM(AK16:AL16)-BJ16</f>
         <v>0.89459382151029843</v>
       </c>
-      <c r="BL16" s="83">
+      <c r="BL16" s="82">
         <f>AM16+(AN16*BE16)</f>
         <v>42.416440294303193</v>
       </c>
-      <c r="BM16" s="84">
+      <c r="BM16" s="83">
         <f>SUM(AM16:AN16)-BL16</f>
         <v>18.583559705696807</v>
       </c>
-      <c r="BN16" s="83">
+      <c r="BN16" s="82">
         <f>SUM(AO16:AP16)*BF16</f>
         <v>0.59544827586206894</v>
       </c>
-      <c r="BO16" s="84">
+      <c r="BO16" s="83">
         <f>SUM(AO16:AP16)-BN16</f>
         <v>0.40455172413793106</v>
       </c>
@@ -8942,37 +8973,37 @@
       <c r="AR17" s="50">
         <v>0</v>
       </c>
-      <c r="AS17" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT17" s="66">
+      <c r="AS17" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="65">
         <v>29</v>
       </c>
-      <c r="AU17" s="66">
+      <c r="AU17" s="65">
         <v>166</v>
       </c>
-      <c r="AV17" s="66">
+      <c r="AV17" s="65">
         <v>26</v>
       </c>
       <c r="AW17" s="35">
         <v>0</v>
       </c>
-      <c r="AX17" s="69" t="s">
+      <c r="AX17" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="AY17" s="70">
+      <c r="AY17" s="69">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AZ17" s="70">
+      <c r="AZ17" s="69">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="BA17" s="70">
+      <c r="BA17" s="69">
         <f t="shared" ref="BA17:BA19" si="17">AO17/SUM(AO17:AP17)</f>
         <v>0</v>
       </c>
-      <c r="BB17" s="77" t="s">
+      <c r="BB17" s="76" t="s">
         <v>67</v>
       </c>
       <c r="BC17" s="32" t="str">
@@ -8991,7 +9022,7 @@
         <f>BF15*G17/G15</f>
         <v>0.55009905956112859</v>
       </c>
-      <c r="BG17" s="74" t="s">
+      <c r="BG17" s="73" t="s">
         <v>67</v>
       </c>
       <c r="BH17" s="33">
@@ -9000,34 +9031,34 @@
       <c r="BI17" s="34">
         <v>0</v>
       </c>
-      <c r="BJ17" s="83">
+      <c r="BJ17" s="82">
         <f>SUM(AK17:AL17)*BD17</f>
         <v>22.807675016829265</v>
       </c>
-      <c r="BK17" s="84">
+      <c r="BK17" s="83">
         <f>SUM(AK17:AL17)-BJ17</f>
         <v>5.1923249831707352</v>
       </c>
-      <c r="BL17" s="83">
+      <c r="BL17" s="82">
         <f>SUM(AM17:AN17)*BE17</f>
         <v>149.99334952840741</v>
       </c>
-      <c r="BM17" s="84">
+      <c r="BM17" s="83">
         <f>SUM(AM17:AN17)-BL17</f>
         <v>14.006650471592593</v>
       </c>
-      <c r="BN17" s="83">
+      <c r="BN17" s="82">
         <f>SUM(AO17:AP17)*BF17</f>
         <v>14.302575548589344</v>
       </c>
-      <c r="BO17" s="84">
+      <c r="BO17" s="83">
         <f>SUM(AO17:AP17)-BN17</f>
         <v>11.697424451410656</v>
       </c>
-      <c r="BP17" s="83">
-        <v>0</v>
-      </c>
-      <c r="BQ17" s="85">
+      <c r="BP17" s="82">
+        <v>0</v>
+      </c>
+      <c r="BQ17" s="84">
         <v>0</v>
       </c>
     </row>
@@ -9045,7 +9076,7 @@
       <c r="D18" s="21">
         <v>184597</v>
       </c>
-      <c r="E18" s="76">
+      <c r="E18" s="75">
         <v>66794</v>
       </c>
       <c r="F18" s="44">
@@ -9172,37 +9203,37 @@
       <c r="AR18" s="52">
         <v>0</v>
       </c>
-      <c r="AS18" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT18" s="66">
+      <c r="AS18" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="65">
         <v>19</v>
       </c>
-      <c r="AU18" s="66">
+      <c r="AU18" s="65">
         <v>182</v>
       </c>
-      <c r="AV18" s="66">
+      <c r="AV18" s="65">
         <v>21</v>
       </c>
       <c r="AW18" s="35">
         <v>0</v>
       </c>
-      <c r="AX18" s="69" t="s">
+      <c r="AX18" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="AY18" s="69">
+      <c r="AY18" s="68">
         <f>AK18/SUM(AK18:AL18)</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="AZ18" s="70">
+      <c r="AZ18" s="69">
         <f t="shared" si="16"/>
         <v>0.36464088397790057</v>
       </c>
-      <c r="BA18" s="70">
+      <c r="BA18" s="69">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="BB18" s="77" t="s">
+      <c r="BB18" s="76" t="s">
         <v>67</v>
       </c>
       <c r="BC18" s="32" t="str">
@@ -9221,7 +9252,7 @@
         <f>SUM(BF12*G12+BF15*G15)/SUM(G12,G15)</f>
         <v>0.84831751509922348</v>
       </c>
-      <c r="BG18" s="74" t="s">
+      <c r="BG18" s="73" t="s">
         <v>67</v>
       </c>
       <c r="BH18" s="33">
@@ -9238,26 +9269,26 @@
         <f>AL18</f>
         <v>8</v>
       </c>
-      <c r="BL18" s="83">
+      <c r="BL18" s="82">
         <f>SUM(AM18:AN18)*BE18</f>
         <v>140.13638222270041</v>
       </c>
-      <c r="BM18" s="84">
+      <c r="BM18" s="83">
         <f>SUM(AM18:AN18)-BL18</f>
         <v>40.863617777299595</v>
       </c>
-      <c r="BN18" s="83">
+      <c r="BN18" s="82">
         <f>SUM(AO18:AP18)*BF18</f>
         <v>16.96635030198447</v>
       </c>
-      <c r="BO18" s="84">
+      <c r="BO18" s="83">
         <f>SUM(AO18:AP18)-BN18</f>
         <v>3.0336496980155303</v>
       </c>
-      <c r="BP18" s="83">
-        <v>0</v>
-      </c>
-      <c r="BQ18" s="85">
+      <c r="BP18" s="82">
+        <v>0</v>
+      </c>
+      <c r="BQ18" s="84">
         <v>0</v>
       </c>
     </row>
@@ -9275,7 +9306,7 @@
       <c r="D19" s="44">
         <v>422512</v>
       </c>
-      <c r="E19" s="76">
+      <c r="E19" s="75">
         <v>184597</v>
       </c>
       <c r="F19" s="21">
@@ -9370,7 +9401,7 @@
       <c r="AG19" s="32">
         <v>0.16825396825396827</v>
       </c>
-      <c r="AH19" s="80">
+      <c r="AH19" s="79">
         <v>3.1746031746031746E-3</v>
       </c>
       <c r="AI19" s="46">
@@ -9408,37 +9439,37 @@
       <c r="AR19" s="52">
         <v>1</v>
       </c>
-      <c r="AS19" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT19" s="66">
+      <c r="AS19" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="65">
         <v>134</v>
       </c>
-      <c r="AU19" s="66">
+      <c r="AU19" s="65">
         <v>127</v>
       </c>
-      <c r="AV19" s="66">
+      <c r="AV19" s="65">
         <v>52</v>
       </c>
       <c r="AW19" s="35">
         <v>1</v>
       </c>
-      <c r="AX19" s="70" t="s">
+      <c r="AX19" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="AY19" s="69">
+      <c r="AY19" s="68">
         <f>AK19/SUM(AK19:AL19)</f>
         <v>0.66400000000000003</v>
       </c>
-      <c r="AZ19" s="69">
+      <c r="AZ19" s="68">
         <f>AM19/SUM(AM19:AN19)</f>
         <v>0.61467889908256879</v>
       </c>
-      <c r="BA19" s="70">
+      <c r="BA19" s="69">
         <f t="shared" si="17"/>
         <v>0.23404255319148937</v>
       </c>
-      <c r="BB19" s="77">
+      <c r="BB19" s="76">
         <f>AQ19/SUM(AQ19:AR19)</f>
         <v>0</v>
       </c>
@@ -9457,13 +9488,13 @@
         <f>BF15*G19/G15</f>
         <v>0.62670595611285274</v>
       </c>
-      <c r="BG19" s="74">
-        <v>0</v>
-      </c>
-      <c r="BH19" s="83">
-        <v>0</v>
-      </c>
-      <c r="BI19" s="84">
+      <c r="BG19" s="73">
+        <v>0</v>
+      </c>
+      <c r="BH19" s="82">
+        <v>0</v>
+      </c>
+      <c r="BI19" s="83">
         <v>0</v>
       </c>
       <c r="BJ19" s="33">
@@ -9482,19 +9513,19 @@
         <f>AN19</f>
         <v>42</v>
       </c>
-      <c r="BN19" s="83">
+      <c r="BN19" s="82">
         <f>SUM(AO19:AP19)*BF19</f>
         <v>29.455179937304077</v>
       </c>
-      <c r="BO19" s="84">
+      <c r="BO19" s="83">
         <f>SUM(AO19:AP19)-BN19</f>
         <v>17.544820062695923</v>
       </c>
-      <c r="BP19" s="83">
+      <c r="BP19" s="82">
         <f>SUM(AQ19:AR19)*BG19</f>
         <v>0</v>
       </c>
-      <c r="BQ19" s="85">
+      <c r="BQ19" s="84">
         <f>SUM(AQ19:AR19)-BP19</f>
         <v>1</v>
       </c>
@@ -9607,41 +9638,123 @@
       <c r="AH20" s="26">
         <v>0</v>
       </c>
-      <c r="AI20" s="33"/>
-      <c r="AJ20" s="34"/>
-      <c r="AK20" s="46"/>
-      <c r="AL20" s="47"/>
-      <c r="AM20" s="33"/>
-      <c r="AN20" s="34"/>
-      <c r="AO20" s="33"/>
-      <c r="AP20" s="34"/>
-      <c r="AQ20" s="46"/>
-      <c r="AR20" s="52"/>
-      <c r="AS20" s="65"/>
-      <c r="AT20" s="66"/>
-      <c r="AU20" s="66"/>
-      <c r="AV20" s="66"/>
-      <c r="AW20" s="35"/>
-      <c r="AX20" s="40"/>
-      <c r="AY20" s="53"/>
-      <c r="AZ20" s="42"/>
-      <c r="BA20" s="42"/>
-      <c r="BB20" s="43"/>
-      <c r="BC20" s="32"/>
-      <c r="BD20" s="32"/>
-      <c r="BE20" s="32"/>
-      <c r="BF20" s="32"/>
-      <c r="BG20" s="26"/>
-      <c r="BH20" s="33"/>
-      <c r="BI20" s="34"/>
-      <c r="BJ20" s="46"/>
-      <c r="BK20" s="47"/>
-      <c r="BL20" s="33"/>
-      <c r="BM20" s="34"/>
-      <c r="BN20" s="33"/>
-      <c r="BO20" s="34"/>
-      <c r="BP20" s="46"/>
-      <c r="BQ20" s="52"/>
+      <c r="AI20" s="102">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="103">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="46">
+        <v>1</v>
+      </c>
+      <c r="AL20" s="47">
+        <v>48</v>
+      </c>
+      <c r="AM20" s="33">
+        <v>135</v>
+      </c>
+      <c r="AN20" s="34">
+        <v>8</v>
+      </c>
+      <c r="AO20" s="33">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="34">
+        <v>2</v>
+      </c>
+      <c r="AQ20" s="46">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="52">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="65">
+        <v>49</v>
+      </c>
+      <c r="AU20" s="65">
+        <v>143</v>
+      </c>
+      <c r="AV20" s="65">
+        <v>2</v>
+      </c>
+      <c r="AW20" s="35">
+        <v>0</v>
+      </c>
+      <c r="AX20" s="104" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY20" s="69">
+        <f>AK20/AT20</f>
+        <v>2.0408163265306121E-2</v>
+      </c>
+      <c r="AZ20" s="68">
+        <f>AM20/AU20</f>
+        <v>0.94405594405594406</v>
+      </c>
+      <c r="BA20" s="68">
+        <f>AO20/AV20</f>
+        <v>0</v>
+      </c>
+      <c r="BB20" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="BC20" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD20" s="49">
+        <f>AVERAGE(BD14:BD17,BD11)</f>
+        <v>0.8228046628843344</v>
+      </c>
+      <c r="BE20" s="32">
+        <f>AZ20</f>
+        <v>0.94405594405594406</v>
+      </c>
+      <c r="BF20" s="32">
+        <f>BF16*G20/G16</f>
+        <v>0.16750846394984323</v>
+      </c>
+      <c r="BG20" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH20" s="109">
+        <v>0</v>
+      </c>
+      <c r="BI20" s="110">
+        <v>0</v>
+      </c>
+      <c r="BJ20" s="100">
+        <f>SUM(AK20:AL20)*BD20</f>
+        <v>40.317428481332385</v>
+      </c>
+      <c r="BK20" s="101">
+        <f>SUM(AK20:AL20)-BJ20</f>
+        <v>8.6825715186676149</v>
+      </c>
+      <c r="BL20" s="33">
+        <f>AM20</f>
+        <v>135</v>
+      </c>
+      <c r="BM20" s="34">
+        <f>AN20</f>
+        <v>8</v>
+      </c>
+      <c r="BN20" s="82">
+        <f>SUM(AO20:AP20)*BF20</f>
+        <v>0.33501692789968646</v>
+      </c>
+      <c r="BO20" s="83">
+        <f>SUM(AO20:AP20)-BN20</f>
+        <v>1.6649830721003136</v>
+      </c>
+      <c r="BP20" s="82">
+        <v>0</v>
+      </c>
+      <c r="BQ20" s="84">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:69" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="21">
@@ -9720,22 +9833,22 @@
       <c r="AH21" s="26"/>
       <c r="AI21" s="33"/>
       <c r="AJ21" s="34"/>
-      <c r="AK21" s="33"/>
-      <c r="AL21" s="34"/>
+      <c r="AK21" s="102"/>
+      <c r="AL21" s="103"/>
       <c r="AM21" s="46"/>
       <c r="AN21" s="47"/>
       <c r="AO21" s="33"/>
       <c r="AP21" s="34"/>
       <c r="AQ21" s="33"/>
       <c r="AR21" s="35"/>
-      <c r="AS21" s="65"/>
-      <c r="AT21" s="66"/>
-      <c r="AU21" s="66"/>
-      <c r="AV21" s="66"/>
+      <c r="AS21" s="64"/>
+      <c r="AT21" s="65"/>
+      <c r="AU21" s="65"/>
+      <c r="AV21" s="65"/>
       <c r="AW21" s="35"/>
       <c r="AX21" s="21"/>
-      <c r="AY21" s="21"/>
-      <c r="AZ21" s="54"/>
+      <c r="AY21" s="105"/>
+      <c r="AZ21" s="53"/>
       <c r="BB21" s="36"/>
       <c r="BC21" s="32"/>
       <c r="BD21" s="32"/>
@@ -9744,8 +9857,8 @@
       <c r="BG21" s="26"/>
       <c r="BH21" s="33"/>
       <c r="BI21" s="34"/>
-      <c r="BJ21" s="33"/>
-      <c r="BK21" s="34"/>
+      <c r="BJ21" s="106"/>
+      <c r="BK21" s="107"/>
       <c r="BL21" s="46"/>
       <c r="BM21" s="47"/>
       <c r="BN21" s="33"/>
@@ -9774,7 +9887,7 @@
       </c>
       <c r="I22" s="24"/>
       <c r="J22" s="25"/>
-      <c r="K22" s="55"/>
+      <c r="K22" s="54"/>
       <c r="L22" s="25"/>
       <c r="M22" s="23"/>
       <c r="N22" s="27"/>
@@ -9810,20 +9923,21 @@
       <c r="AJ22" s="34"/>
       <c r="AK22" s="33"/>
       <c r="AL22" s="34"/>
-      <c r="AM22" s="33"/>
-      <c r="AN22" s="34"/>
+      <c r="AM22" s="102"/>
+      <c r="AN22" s="103"/>
       <c r="AO22" s="46"/>
       <c r="AP22" s="47"/>
       <c r="AQ22" s="33"/>
       <c r="AR22" s="35"/>
-      <c r="AS22" s="65"/>
-      <c r="AT22" s="66"/>
-      <c r="AU22" s="66"/>
-      <c r="AV22" s="66"/>
+      <c r="AS22" s="64"/>
+      <c r="AT22" s="65"/>
+      <c r="AU22" s="65"/>
+      <c r="AV22" s="65"/>
       <c r="AW22" s="35"/>
       <c r="AX22" s="21"/>
       <c r="AY22" s="21"/>
-      <c r="BA22" s="54"/>
+      <c r="AZ22" s="105"/>
+      <c r="BA22" s="53"/>
       <c r="BB22" s="36"/>
       <c r="BC22" s="32"/>
       <c r="BD22" s="32"/>
@@ -9834,8 +9948,8 @@
       <c r="BI22" s="34"/>
       <c r="BJ22" s="33"/>
       <c r="BK22" s="34"/>
-      <c r="BL22" s="33"/>
-      <c r="BM22" s="34"/>
+      <c r="BL22" s="106"/>
+      <c r="BM22" s="107"/>
       <c r="BN22" s="46"/>
       <c r="BO22" s="47"/>
       <c r="BP22" s="33"/>
@@ -9896,18 +10010,19 @@
       <c r="AL23" s="34"/>
       <c r="AM23" s="33"/>
       <c r="AN23" s="34"/>
-      <c r="AO23" s="33"/>
-      <c r="AP23" s="34"/>
+      <c r="AO23" s="102"/>
+      <c r="AP23" s="103"/>
       <c r="AQ23" s="46"/>
       <c r="AR23" s="52"/>
-      <c r="AS23" s="65"/>
-      <c r="AT23" s="66"/>
-      <c r="AU23" s="66"/>
-      <c r="AV23" s="66"/>
+      <c r="AS23" s="64"/>
+      <c r="AT23" s="65"/>
+      <c r="AU23" s="65"/>
+      <c r="AV23" s="65"/>
       <c r="AW23" s="35"/>
       <c r="AX23" s="21"/>
       <c r="AY23" s="21"/>
-      <c r="BB23" s="56"/>
+      <c r="BA23" s="105"/>
+      <c r="BB23" s="55"/>
       <c r="BG23" s="36"/>
       <c r="BH23" s="33"/>
       <c r="BI23" s="34"/>
@@ -9915,8 +10030,8 @@
       <c r="BK23" s="34"/>
       <c r="BL23" s="33"/>
       <c r="BM23" s="34"/>
-      <c r="BN23" s="33"/>
-      <c r="BO23" s="34"/>
+      <c r="BN23" s="106"/>
+      <c r="BO23" s="107"/>
       <c r="BP23" s="46"/>
       <c r="BQ23" s="52"/>
     </row>
@@ -9932,7 +10047,7 @@
       <c r="G24" s="21">
         <v>478224</v>
       </c>
-      <c r="H24" s="57">
+      <c r="H24" s="56">
         <v>500039</v>
       </c>
       <c r="I24" s="27"/>
@@ -9971,16 +10086,16 @@
       <c r="AN24" s="34"/>
       <c r="AO24" s="33"/>
       <c r="AP24" s="34"/>
-      <c r="AQ24" s="33"/>
-      <c r="AR24" s="35"/>
-      <c r="AS24" s="65"/>
-      <c r="AT24" s="66"/>
-      <c r="AU24" s="66"/>
-      <c r="AV24" s="66"/>
+      <c r="AQ24" s="102"/>
+      <c r="AR24" s="103"/>
+      <c r="AS24" s="64"/>
+      <c r="AT24" s="65"/>
+      <c r="AU24" s="65"/>
+      <c r="AV24" s="65"/>
       <c r="AW24" s="35"/>
       <c r="AX24" s="21"/>
       <c r="AY24" s="21"/>
-      <c r="BB24" s="36"/>
+      <c r="BB24" s="105"/>
       <c r="BG24" s="36"/>
       <c r="BH24" s="33"/>
       <c r="BI24" s="34"/>
@@ -9990,11 +10105,11 @@
       <c r="BM24" s="34"/>
       <c r="BN24" s="33"/>
       <c r="BO24" s="34"/>
-      <c r="BP24" s="33"/>
-      <c r="BQ24" s="35"/>
+      <c r="BP24" s="106"/>
+      <c r="BQ24" s="108"/>
     </row>
     <row r="25" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="BM25" s="86"/>
+      <c r="BM25" s="85"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P9:R9 N9:N12 P13:R14 Q10:R10 P11 R11 P12:Q12 P20:Q20 R16 P19 Q15:R15 N17:N18">

</xml_diff>